<commit_message>
Added more for 10 reference testing
</commit_message>
<xml_diff>
--- a/GHT/validation_set_results.xlsx
+++ b/GHT/validation_set_results.xlsx
@@ -291,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -322,7 +322,6 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -355,8 +354,12 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,10 +661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J85"/>
+  <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="J65" sqref="J65"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,16 +679,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="35"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="34"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -712,7 +715,7 @@
       <c r="H2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="22" t="s">
         <v>12</v>
       </c>
     </row>
@@ -793,7 +796,7 @@
       <c r="F5" s="8">
         <v>0.5</v>
       </c>
-      <c r="G5" s="27">
+      <c r="G5" s="26">
         <v>1373</v>
       </c>
       <c r="H5" s="10">
@@ -923,10 +926,10 @@
       <c r="F10" s="13">
         <v>0.5</v>
       </c>
-      <c r="G10" s="29">
+      <c r="G10" s="28">
         <v>1129</v>
       </c>
-      <c r="H10" s="30">
+      <c r="H10" s="29">
         <v>90</v>
       </c>
     </row>
@@ -1053,10 +1056,10 @@
       <c r="F15" s="8">
         <v>0.5</v>
       </c>
-      <c r="G15" s="29">
+      <c r="G15" s="28">
         <v>1130</v>
       </c>
-      <c r="H15" s="30">
+      <c r="H15" s="29">
         <v>90</v>
       </c>
     </row>
@@ -1183,7 +1186,7 @@
       <c r="F20" s="13">
         <v>0.5</v>
       </c>
-      <c r="G20" s="28">
+      <c r="G20" s="27">
         <v>1139</v>
       </c>
       <c r="H20" s="21">
@@ -1346,16 +1349,16 @@
     </row>
     <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="36" t="s">
+      <c r="A30" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="37"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="37"/>
-      <c r="H30" s="38"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="37"/>
       <c r="J30" t="s">
         <v>11</v>
       </c>
@@ -1445,7 +1448,7 @@
       <c r="B34" s="8">
         <v>20</v>
       </c>
-      <c r="C34" s="24">
+      <c r="C34" s="23">
         <v>180</v>
       </c>
       <c r="D34" s="9">
@@ -1471,7 +1474,7 @@
       <c r="B35" s="8">
         <v>20</v>
       </c>
-      <c r="C35" s="24">
+      <c r="C35" s="23">
         <v>200</v>
       </c>
       <c r="D35" s="9">
@@ -1497,7 +1500,7 @@
       <c r="B36" s="8">
         <v>20</v>
       </c>
-      <c r="C36" s="24">
+      <c r="C36" s="23">
         <v>220</v>
       </c>
       <c r="D36" s="9">
@@ -1523,7 +1526,7 @@
       <c r="B37" s="13">
         <v>30</v>
       </c>
-      <c r="C37" s="25">
+      <c r="C37" s="24">
         <v>140</v>
       </c>
       <c r="D37" s="14">
@@ -1549,7 +1552,7 @@
       <c r="B38" s="13">
         <v>30</v>
       </c>
-      <c r="C38" s="25">
+      <c r="C38" s="24">
         <v>160</v>
       </c>
       <c r="D38" s="14">
@@ -1575,7 +1578,7 @@
       <c r="B39" s="13">
         <v>30</v>
       </c>
-      <c r="C39" s="25">
+      <c r="C39" s="24">
         <v>180</v>
       </c>
       <c r="D39" s="14">
@@ -1601,7 +1604,7 @@
       <c r="B40" s="13">
         <v>30</v>
       </c>
-      <c r="C40" s="25">
+      <c r="C40" s="24">
         <v>200</v>
       </c>
       <c r="D40" s="14">
@@ -1627,7 +1630,7 @@
       <c r="B41" s="13">
         <v>30</v>
       </c>
-      <c r="C41" s="25">
+      <c r="C41" s="24">
         <v>220</v>
       </c>
       <c r="D41" s="14">
@@ -1649,7 +1652,7 @@
       <c r="B42" s="8">
         <v>40</v>
       </c>
-      <c r="C42" s="24">
+      <c r="C42" s="23">
         <v>140</v>
       </c>
       <c r="D42" s="9">
@@ -1671,7 +1674,7 @@
       <c r="B43" s="8">
         <v>40</v>
       </c>
-      <c r="C43" s="24">
+      <c r="C43" s="23">
         <v>160</v>
       </c>
       <c r="D43" s="9">
@@ -1693,7 +1696,7 @@
       <c r="B44" s="8">
         <v>40</v>
       </c>
-      <c r="C44" s="24">
+      <c r="C44" s="23">
         <v>180</v>
       </c>
       <c r="D44" s="9">
@@ -1715,7 +1718,7 @@
       <c r="B45" s="8">
         <v>40</v>
       </c>
-      <c r="C45" s="24">
+      <c r="C45" s="23">
         <v>200</v>
       </c>
       <c r="D45" s="9">
@@ -1737,7 +1740,7 @@
       <c r="B46" s="8">
         <v>40</v>
       </c>
-      <c r="C46" s="24">
+      <c r="C46" s="23">
         <v>220</v>
       </c>
       <c r="D46" s="9">
@@ -1759,7 +1762,7 @@
       <c r="B47" s="13">
         <v>50</v>
       </c>
-      <c r="C47" s="25">
+      <c r="C47" s="24">
         <v>140</v>
       </c>
       <c r="D47" s="14">
@@ -1781,7 +1784,7 @@
       <c r="B48" s="13">
         <v>50</v>
       </c>
-      <c r="C48" s="25">
+      <c r="C48" s="24">
         <v>160</v>
       </c>
       <c r="D48" s="14">
@@ -1803,7 +1806,7 @@
       <c r="B49" s="13">
         <v>50</v>
       </c>
-      <c r="C49" s="25">
+      <c r="C49" s="24">
         <v>180</v>
       </c>
       <c r="D49" s="14">
@@ -1825,7 +1828,7 @@
       <c r="B50" s="13">
         <v>50</v>
       </c>
-      <c r="C50" s="25">
+      <c r="C50" s="24">
         <v>200</v>
       </c>
       <c r="D50" s="14">
@@ -1847,7 +1850,7 @@
       <c r="B51" s="13">
         <v>50</v>
       </c>
-      <c r="C51" s="25">
+      <c r="C51" s="24">
         <v>220</v>
       </c>
       <c r="D51" s="14">
@@ -1869,7 +1872,7 @@
       <c r="B52" s="8">
         <v>60</v>
       </c>
-      <c r="C52" s="24">
+      <c r="C52" s="23">
         <v>140</v>
       </c>
       <c r="D52" s="9">
@@ -1891,7 +1894,7 @@
       <c r="B53" s="8">
         <v>60</v>
       </c>
-      <c r="C53" s="24">
+      <c r="C53" s="23">
         <v>160</v>
       </c>
       <c r="D53" s="9">
@@ -1913,7 +1916,7 @@
       <c r="B54" s="8">
         <v>60</v>
       </c>
-      <c r="C54" s="24">
+      <c r="C54" s="23">
         <v>180</v>
       </c>
       <c r="D54" s="9">
@@ -1935,7 +1938,7 @@
       <c r="B55" s="8">
         <v>60</v>
       </c>
-      <c r="C55" s="24">
+      <c r="C55" s="23">
         <v>200</v>
       </c>
       <c r="D55" s="9">
@@ -1957,7 +1960,7 @@
       <c r="B56" s="18">
         <v>60</v>
       </c>
-      <c r="C56" s="26">
+      <c r="C56" s="25">
         <v>220</v>
       </c>
       <c r="D56" s="19">
@@ -1974,16 +1977,16 @@
     </row>
     <row r="58" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="33" t="s">
+      <c r="A59" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B59" s="34"/>
-      <c r="C59" s="34"/>
-      <c r="D59" s="34"/>
-      <c r="E59" s="34"/>
-      <c r="F59" s="34"/>
-      <c r="G59" s="34"/>
-      <c r="H59" s="35"/>
+      <c r="B59" s="33"/>
+      <c r="C59" s="33"/>
+      <c r="D59" s="33"/>
+      <c r="E59" s="33"/>
+      <c r="F59" s="33"/>
+      <c r="G59" s="33"/>
+      <c r="H59" s="34"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
@@ -2012,102 +2015,118 @@
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="7">
+      <c r="A61" s="12">
         <v>10</v>
       </c>
-      <c r="B61" s="8">
-        <v>20</v>
+      <c r="B61" s="13">
+        <v>30</v>
       </c>
       <c r="C61" s="24">
+        <v>120</v>
+      </c>
+      <c r="D61" s="14">
+        <v>1</v>
+      </c>
+      <c r="E61" s="14">
+        <v>0</v>
+      </c>
+      <c r="F61" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G61" s="30">
+        <v>1305</v>
+      </c>
+      <c r="H61" s="31">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="12">
+        <v>10</v>
+      </c>
+      <c r="B62" s="13">
+        <v>30</v>
+      </c>
+      <c r="C62" s="24">
         <v>140</v>
       </c>
-      <c r="D61" s="9">
-        <v>1</v>
-      </c>
-      <c r="E61" s="9">
-        <v>0</v>
-      </c>
-      <c r="F61" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G61" s="39"/>
-      <c r="H61" s="40"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="7">
+      <c r="D62" s="14">
+        <v>1</v>
+      </c>
+      <c r="E62" s="14">
+        <v>0</v>
+      </c>
+      <c r="F62" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G62" s="30">
+        <v>1090</v>
+      </c>
+      <c r="H62" s="31">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="12">
         <v>10</v>
       </c>
-      <c r="B62" s="8">
-        <v>20</v>
-      </c>
-      <c r="C62" s="24">
+      <c r="B63" s="13">
+        <v>30</v>
+      </c>
+      <c r="C63" s="24">
         <v>160</v>
       </c>
-      <c r="D62" s="9">
-        <v>1</v>
-      </c>
-      <c r="E62" s="9">
-        <v>0</v>
-      </c>
-      <c r="F62" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G62" s="39"/>
-      <c r="H62" s="40"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="7">
+      <c r="D63" s="14">
+        <v>1</v>
+      </c>
+      <c r="E63" s="14">
+        <v>0</v>
+      </c>
+      <c r="F63" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G63" s="30">
+        <v>1402</v>
+      </c>
+      <c r="H63" s="31">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="12">
         <v>10</v>
       </c>
-      <c r="B63" s="8">
-        <v>20</v>
-      </c>
-      <c r="C63" s="24">
+      <c r="B64" s="13">
+        <v>30</v>
+      </c>
+      <c r="C64" s="24">
         <v>180</v>
       </c>
-      <c r="D63" s="9">
-        <v>1</v>
-      </c>
-      <c r="E63" s="9">
-        <v>0</v>
-      </c>
-      <c r="F63" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G63" s="39"/>
-      <c r="H63" s="40"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="7">
-        <v>10</v>
-      </c>
-      <c r="B64" s="8">
-        <v>20</v>
-      </c>
-      <c r="C64" s="24">
-        <v>200</v>
-      </c>
-      <c r="D64" s="9">
-        <v>1</v>
-      </c>
-      <c r="E64" s="9">
-        <v>0</v>
-      </c>
-      <c r="F64" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G64" s="39"/>
-      <c r="H64" s="40"/>
+      <c r="D64" s="14">
+        <v>1</v>
+      </c>
+      <c r="E64" s="14">
+        <v>0</v>
+      </c>
+      <c r="F64" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G64" s="30">
+        <v>1191</v>
+      </c>
+      <c r="H64" s="31">
+        <v>90</v>
+      </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="7">
         <v>10</v>
       </c>
       <c r="B65" s="8">
-        <v>20</v>
-      </c>
-      <c r="C65" s="24">
-        <v>220</v>
+        <v>40</v>
+      </c>
+      <c r="C65" s="23">
+        <v>120</v>
       </c>
       <c r="D65" s="9">
         <v>1</v>
@@ -2118,84 +2137,88 @@
       <c r="F65" s="8">
         <v>0.5</v>
       </c>
-      <c r="G65" s="39"/>
-      <c r="H65" s="40"/>
+      <c r="G65" s="38">
+        <v>2017</v>
+      </c>
+      <c r="H65" s="39">
+        <v>93</v>
+      </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="12">
+      <c r="A66" s="7">
         <v>10</v>
       </c>
-      <c r="B66" s="13">
-        <v>30</v>
-      </c>
-      <c r="C66" s="25">
-        <v>120</v>
-      </c>
-      <c r="D66" s="14">
-        <v>1</v>
-      </c>
-      <c r="E66" s="14">
-        <v>0</v>
-      </c>
-      <c r="F66" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="G66" s="31">
-        <v>1305</v>
-      </c>
-      <c r="H66" s="32">
-        <v>92</v>
+      <c r="B66" s="8">
+        <v>40</v>
+      </c>
+      <c r="C66" s="23">
+        <v>140</v>
+      </c>
+      <c r="D66" s="9">
+        <v>1</v>
+      </c>
+      <c r="E66" s="9">
+        <v>0</v>
+      </c>
+      <c r="F66" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G66" s="28">
+        <v>874</v>
+      </c>
+      <c r="H66" s="29">
+        <v>97</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="12">
+      <c r="A67" s="7">
         <v>10</v>
       </c>
-      <c r="B67" s="13">
-        <v>30</v>
-      </c>
-      <c r="C67" s="25">
-        <v>140</v>
-      </c>
-      <c r="D67" s="14">
-        <v>1</v>
-      </c>
-      <c r="E67" s="14">
-        <v>0</v>
-      </c>
-      <c r="F67" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="G67" s="31">
-        <v>1090</v>
-      </c>
-      <c r="H67" s="32">
-        <v>94</v>
+      <c r="B67" s="8">
+        <v>40</v>
+      </c>
+      <c r="C67" s="23">
+        <v>160</v>
+      </c>
+      <c r="D67" s="9">
+        <v>1</v>
+      </c>
+      <c r="E67" s="9">
+        <v>0</v>
+      </c>
+      <c r="F67" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G67" s="38">
+        <v>1098</v>
+      </c>
+      <c r="H67" s="39">
+        <v>93</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="12">
+      <c r="A68" s="7">
         <v>10</v>
       </c>
-      <c r="B68" s="13">
-        <v>30</v>
-      </c>
-      <c r="C68" s="25">
-        <v>160</v>
-      </c>
-      <c r="D68" s="14">
-        <v>1</v>
-      </c>
-      <c r="E68" s="14">
-        <v>0</v>
-      </c>
-      <c r="F68" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="G68" s="31">
-        <v>1402</v>
-      </c>
-      <c r="H68" s="32">
+      <c r="B68" s="8">
+        <v>40</v>
+      </c>
+      <c r="C68" s="23">
+        <v>180</v>
+      </c>
+      <c r="D68" s="9">
+        <v>1</v>
+      </c>
+      <c r="E68" s="9">
+        <v>0</v>
+      </c>
+      <c r="F68" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G68" s="38">
+        <v>924</v>
+      </c>
+      <c r="H68" s="39">
         <v>91</v>
       </c>
     </row>
@@ -2204,10 +2227,10 @@
         <v>10</v>
       </c>
       <c r="B69" s="13">
-        <v>30</v>
-      </c>
-      <c r="C69" s="25">
-        <v>180</v>
+        <v>50</v>
+      </c>
+      <c r="C69" s="24">
+        <v>120</v>
       </c>
       <c r="D69" s="14">
         <v>1</v>
@@ -2218,11 +2241,11 @@
       <c r="F69" s="13">
         <v>0.5</v>
       </c>
-      <c r="G69" s="31">
-        <v>1191</v>
-      </c>
-      <c r="H69" s="32">
-        <v>90</v>
+      <c r="G69" s="30">
+        <v>2009</v>
+      </c>
+      <c r="H69" s="31">
+        <v>94</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -2230,10 +2253,10 @@
         <v>10</v>
       </c>
       <c r="B70" s="13">
-        <v>30</v>
-      </c>
-      <c r="C70" s="25">
-        <v>200</v>
+        <v>50</v>
+      </c>
+      <c r="C70" s="24">
+        <v>140</v>
       </c>
       <c r="D70" s="14">
         <v>1</v>
@@ -2244,354 +2267,64 @@
       <c r="F70" s="13">
         <v>0.5</v>
       </c>
-      <c r="G70" s="31">
-        <v>1344</v>
-      </c>
-      <c r="H70" s="32">
-        <v>88</v>
+      <c r="G70" s="30">
+        <v>986</v>
+      </c>
+      <c r="H70" s="31">
+        <v>95</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="7">
+      <c r="A71" s="12">
         <v>10</v>
       </c>
-      <c r="B71" s="8">
-        <v>40</v>
+      <c r="B71" s="13">
+        <v>50</v>
       </c>
       <c r="C71" s="24">
-        <v>120</v>
-      </c>
-      <c r="D71" s="9">
-        <v>1</v>
-      </c>
-      <c r="E71" s="9">
-        <v>0</v>
-      </c>
-      <c r="F71" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G71" s="39"/>
-      <c r="H71" s="40"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="7">
+        <v>160</v>
+      </c>
+      <c r="D71" s="14">
+        <v>1</v>
+      </c>
+      <c r="E71" s="14">
+        <v>0</v>
+      </c>
+      <c r="F71" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G71" s="28">
+        <v>728</v>
+      </c>
+      <c r="H71" s="29">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="40">
         <v>10</v>
       </c>
-      <c r="B72" s="8">
-        <v>40</v>
-      </c>
-      <c r="C72" s="24">
-        <v>140</v>
-      </c>
-      <c r="D72" s="9">
-        <v>1</v>
-      </c>
-      <c r="E72" s="9">
-        <v>0</v>
-      </c>
-      <c r="F72" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G72" s="27">
-        <v>874</v>
-      </c>
-      <c r="H72" s="22">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="7">
-        <v>10</v>
-      </c>
-      <c r="B73" s="8">
-        <v>40</v>
-      </c>
-      <c r="C73" s="24">
-        <v>160</v>
-      </c>
-      <c r="D73" s="9">
-        <v>1</v>
-      </c>
-      <c r="E73" s="9">
-        <v>0</v>
-      </c>
-      <c r="F73" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G73" s="39">
-        <v>1098</v>
-      </c>
-      <c r="H73" s="40">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="7">
-        <v>10</v>
-      </c>
-      <c r="B74" s="8">
-        <v>40</v>
-      </c>
-      <c r="C74" s="24">
+      <c r="B72" s="41">
+        <v>50</v>
+      </c>
+      <c r="C72" s="42">
         <v>180</v>
       </c>
-      <c r="D74" s="9">
-        <v>1</v>
-      </c>
-      <c r="E74" s="9">
-        <v>0</v>
-      </c>
-      <c r="F74" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G74" s="39">
-        <v>924</v>
-      </c>
-      <c r="H74" s="40">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="7">
-        <v>10</v>
-      </c>
-      <c r="B75" s="8">
-        <v>40</v>
-      </c>
-      <c r="C75" s="24">
-        <v>200</v>
-      </c>
-      <c r="D75" s="9">
-        <v>1</v>
-      </c>
-      <c r="E75" s="9">
-        <v>0</v>
-      </c>
-      <c r="F75" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G75" s="39"/>
-      <c r="H75" s="40"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="12">
-        <v>10</v>
-      </c>
-      <c r="B76" s="13">
-        <v>50</v>
-      </c>
-      <c r="C76" s="25">
-        <v>140</v>
-      </c>
-      <c r="D76" s="14">
-        <v>1</v>
-      </c>
-      <c r="E76" s="14">
-        <v>0</v>
-      </c>
-      <c r="F76" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="G76" s="31"/>
-      <c r="H76" s="32"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="12">
-        <v>10</v>
-      </c>
-      <c r="B77" s="13">
-        <v>50</v>
-      </c>
-      <c r="C77" s="25">
-        <v>160</v>
-      </c>
-      <c r="D77" s="14">
-        <v>1</v>
-      </c>
-      <c r="E77" s="14">
-        <v>0</v>
-      </c>
-      <c r="F77" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="G77" s="31"/>
-      <c r="H77" s="32"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="12">
-        <v>10</v>
-      </c>
-      <c r="B78" s="13">
-        <v>50</v>
-      </c>
-      <c r="C78" s="25">
-        <v>180</v>
-      </c>
-      <c r="D78" s="14">
-        <v>1</v>
-      </c>
-      <c r="E78" s="14">
-        <v>0</v>
-      </c>
-      <c r="F78" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="G78" s="31"/>
-      <c r="H78" s="32"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" s="12">
-        <v>10</v>
-      </c>
-      <c r="B79" s="13">
-        <v>50</v>
-      </c>
-      <c r="C79" s="25">
-        <v>200</v>
-      </c>
-      <c r="D79" s="14">
-        <v>1</v>
-      </c>
-      <c r="E79" s="14">
-        <v>0</v>
-      </c>
-      <c r="F79" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="G79" s="31"/>
-      <c r="H79" s="32"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="12">
-        <v>10</v>
-      </c>
-      <c r="B80" s="13">
-        <v>50</v>
-      </c>
-      <c r="C80" s="25">
-        <v>220</v>
-      </c>
-      <c r="D80" s="14">
-        <v>1</v>
-      </c>
-      <c r="E80" s="14">
-        <v>0</v>
-      </c>
-      <c r="F80" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="G80" s="31"/>
-      <c r="H80" s="32"/>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="7">
-        <v>10</v>
-      </c>
-      <c r="B81" s="8">
-        <v>60</v>
-      </c>
-      <c r="C81" s="24">
-        <v>140</v>
-      </c>
-      <c r="D81" s="9">
-        <v>1</v>
-      </c>
-      <c r="E81" s="9">
-        <v>0</v>
-      </c>
-      <c r="F81" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G81" s="39"/>
-      <c r="H81" s="40"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="7">
-        <v>10</v>
-      </c>
-      <c r="B82" s="8">
-        <v>60</v>
-      </c>
-      <c r="C82" s="24">
-        <v>160</v>
-      </c>
-      <c r="D82" s="9">
-        <v>1</v>
-      </c>
-      <c r="E82" s="9">
-        <v>0</v>
-      </c>
-      <c r="F82" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G82" s="39"/>
-      <c r="H82" s="40"/>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" s="7">
-        <v>10</v>
-      </c>
-      <c r="B83" s="8">
-        <v>60</v>
-      </c>
-      <c r="C83" s="24">
-        <v>180</v>
-      </c>
-      <c r="D83" s="9">
-        <v>1</v>
-      </c>
-      <c r="E83" s="9">
-        <v>0</v>
-      </c>
-      <c r="F83" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G83" s="39"/>
-      <c r="H83" s="40"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="7">
-        <v>10</v>
-      </c>
-      <c r="B84" s="8">
-        <v>60</v>
-      </c>
-      <c r="C84" s="24">
-        <v>200</v>
-      </c>
-      <c r="D84" s="9">
-        <v>1</v>
-      </c>
-      <c r="E84" s="9">
-        <v>0</v>
-      </c>
-      <c r="F84" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G84" s="39"/>
-      <c r="H84" s="40"/>
-    </row>
-    <row r="85" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="7">
-        <v>10</v>
-      </c>
-      <c r="B85" s="18">
-        <v>60</v>
-      </c>
-      <c r="C85" s="26">
-        <v>220</v>
-      </c>
-      <c r="D85" s="19">
-        <v>1</v>
-      </c>
-      <c r="E85" s="19">
-        <v>0</v>
-      </c>
-      <c r="F85" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="G85" s="41"/>
-      <c r="H85" s="42"/>
+      <c r="D72" s="43">
+        <v>1</v>
+      </c>
+      <c r="E72" s="43">
+        <v>0</v>
+      </c>
+      <c r="F72" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="G72" s="44">
+        <v>866</v>
+      </c>
+      <c r="H72" s="45">
+        <v>90</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Making sure that the multiprocessed and non-multiprocessed files have the same algorithms. Updating validation set results to have more validation performance information.
</commit_message>
<xml_diff>
--- a/GHT/validation_set_results.xlsx
+++ b/GHT/validation_set_results.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE93E26-6F72-4046-9930-727D4CC40B53}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Interim Report" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Power 6 Prior + Top 5 Avg" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="14">
   <si>
     <t>Min Canny</t>
   </si>
@@ -56,11 +58,14 @@
   <si>
     <t>First 5 References (7796800, 6268647, 9049401, 6729799, 8476267)</t>
   </si>
+  <si>
+    <t>Validation Set Result for C1 Spine Detection: Power 6 Prior + Top 5 Avg</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -334,6 +339,14 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -352,14 +365,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -369,6 +374,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -417,7 +425,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -450,9 +458,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -485,6 +510,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -660,37 +702,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="G71" sqref="G71"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" style="1" customWidth="1"/>
-    <col min="5" max="6" width="18.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="52.7109375" customWidth="1"/>
+    <col min="2" max="3" width="18.73046875" customWidth="1"/>
+    <col min="4" max="4" width="18.73046875" style="1" customWidth="1"/>
+    <col min="5" max="6" width="18.73046875" customWidth="1"/>
+    <col min="7" max="7" width="15.73046875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.73046875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="52.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A1" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="34"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="42"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
@@ -719,7 +761,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="7">
         <v>5</v>
       </c>
@@ -748,7 +790,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="7">
         <v>5</v>
       </c>
@@ -777,7 +819,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="7">
         <v>5</v>
       </c>
@@ -803,7 +845,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -829,7 +871,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -855,7 +897,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="12">
         <v>5</v>
       </c>
@@ -881,7 +923,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="12">
         <v>5</v>
       </c>
@@ -907,7 +949,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="12">
         <v>5</v>
       </c>
@@ -933,7 +975,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="12">
         <v>5</v>
       </c>
@@ -959,7 +1001,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" s="12">
         <v>5</v>
       </c>
@@ -985,7 +1027,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" s="7">
         <v>5</v>
       </c>
@@ -1011,7 +1053,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" s="7">
         <v>5</v>
       </c>
@@ -1037,7 +1079,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" s="7">
         <v>5</v>
       </c>
@@ -1063,7 +1105,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" s="7">
         <v>5</v>
       </c>
@@ -1089,7 +1131,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" s="7">
         <v>5</v>
       </c>
@@ -1115,7 +1157,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" s="12">
         <v>5</v>
       </c>
@@ -1141,7 +1183,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" s="12">
         <v>5</v>
       </c>
@@ -1167,7 +1209,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" s="12">
         <v>5</v>
       </c>
@@ -1193,7 +1235,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" s="12">
         <v>5</v>
       </c>
@@ -1215,7 +1257,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="15"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" s="12">
         <v>5</v>
       </c>
@@ -1237,7 +1279,7 @@
       <c r="G22" s="14"/>
       <c r="H22" s="15"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" s="7">
         <v>5</v>
       </c>
@@ -1259,7 +1301,7 @@
       <c r="G23" s="9"/>
       <c r="H23" s="10"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" s="7">
         <v>5</v>
       </c>
@@ -1281,7 +1323,7 @@
       <c r="G24" s="9"/>
       <c r="H24" s="10"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" s="7">
         <v>5</v>
       </c>
@@ -1303,7 +1345,7 @@
       <c r="G25" s="9"/>
       <c r="H25" s="10"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" s="7">
         <v>5</v>
       </c>
@@ -1325,7 +1367,7 @@
       <c r="G26" s="9"/>
       <c r="H26" s="10"/>
     </row>
-    <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A27" s="17">
         <v>5</v>
       </c>
@@ -1347,23 +1389,23 @@
       <c r="G27" s="19"/>
       <c r="H27" s="20"/>
     </row>
-    <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="35" t="s">
+    <row r="29" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A30" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="37"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="45"/>
       <c r="J30" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" s="5" t="s">
         <v>8</v>
       </c>
@@ -1389,7 +1431,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32" s="7">
         <v>1</v>
       </c>
@@ -1415,7 +1457,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A33" s="7">
         <v>1</v>
       </c>
@@ -1441,7 +1483,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A34" s="7">
         <v>1</v>
       </c>
@@ -1467,7 +1509,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A35" s="7">
         <v>1</v>
       </c>
@@ -1493,7 +1535,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A36" s="7">
         <v>1</v>
       </c>
@@ -1519,7 +1561,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A37" s="12">
         <v>1</v>
       </c>
@@ -1545,7 +1587,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A38" s="12">
         <v>1</v>
       </c>
@@ -1571,7 +1613,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A39" s="12">
         <v>1</v>
       </c>
@@ -1597,7 +1639,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A40" s="12">
         <v>1</v>
       </c>
@@ -1623,7 +1665,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A41" s="12">
         <v>1</v>
       </c>
@@ -1645,7 +1687,7 @@
       <c r="G41" s="14"/>
       <c r="H41" s="15"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A42" s="7">
         <v>1</v>
       </c>
@@ -1667,7 +1709,7 @@
       <c r="G42" s="9"/>
       <c r="H42" s="10"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A43" s="7">
         <v>1</v>
       </c>
@@ -1689,7 +1731,7 @@
       <c r="G43" s="9"/>
       <c r="H43" s="10"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A44" s="7">
         <v>1</v>
       </c>
@@ -1711,7 +1753,7 @@
       <c r="G44" s="9"/>
       <c r="H44" s="10"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A45" s="7">
         <v>1</v>
       </c>
@@ -1733,7 +1775,7 @@
       <c r="G45" s="9"/>
       <c r="H45" s="10"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A46" s="7">
         <v>1</v>
       </c>
@@ -1755,7 +1797,7 @@
       <c r="G46" s="9"/>
       <c r="H46" s="10"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A47" s="12">
         <v>1</v>
       </c>
@@ -1777,7 +1819,7 @@
       <c r="G47" s="14"/>
       <c r="H47" s="15"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A48" s="12">
         <v>1</v>
       </c>
@@ -1799,7 +1841,7 @@
       <c r="G48" s="14"/>
       <c r="H48" s="15"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A49" s="12">
         <v>1</v>
       </c>
@@ -1821,7 +1863,7 @@
       <c r="G49" s="14"/>
       <c r="H49" s="15"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A50" s="12">
         <v>1</v>
       </c>
@@ -1843,7 +1885,7 @@
       <c r="G50" s="14"/>
       <c r="H50" s="15"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A51" s="12">
         <v>1</v>
       </c>
@@ -1865,7 +1907,7 @@
       <c r="G51" s="14"/>
       <c r="H51" s="15"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A52" s="7">
         <v>1</v>
       </c>
@@ -1887,7 +1929,7 @@
       <c r="G52" s="9"/>
       <c r="H52" s="10"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A53" s="7">
         <v>1</v>
       </c>
@@ -1909,7 +1951,7 @@
       <c r="G53" s="9"/>
       <c r="H53" s="10"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A54" s="7">
         <v>1</v>
       </c>
@@ -1931,7 +1973,7 @@
       <c r="G54" s="9"/>
       <c r="H54" s="10"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A55" s="7">
         <v>1</v>
       </c>
@@ -1953,7 +1995,7 @@
       <c r="G55" s="9"/>
       <c r="H55" s="10"/>
     </row>
-    <row r="56" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A56" s="7">
         <v>1</v>
       </c>
@@ -1975,20 +2017,20 @@
       <c r="G56" s="19"/>
       <c r="H56" s="20"/>
     </row>
-    <row r="58" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="32" t="s">
+    <row r="58" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A59" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B59" s="33"/>
-      <c r="C59" s="33"/>
-      <c r="D59" s="33"/>
-      <c r="E59" s="33"/>
-      <c r="F59" s="33"/>
-      <c r="G59" s="33"/>
-      <c r="H59" s="34"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B59" s="41"/>
+      <c r="C59" s="41"/>
+      <c r="D59" s="41"/>
+      <c r="E59" s="41"/>
+      <c r="F59" s="41"/>
+      <c r="G59" s="41"/>
+      <c r="H59" s="42"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A60" s="5" t="s">
         <v>8</v>
       </c>
@@ -2014,7 +2056,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A61" s="12">
         <v>10</v>
       </c>
@@ -2040,7 +2082,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A62" s="12">
         <v>10</v>
       </c>
@@ -2066,7 +2108,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A63" s="12">
         <v>10</v>
       </c>
@@ -2092,7 +2134,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A64" s="12">
         <v>10</v>
       </c>
@@ -2118,7 +2160,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A65" s="7">
         <v>10</v>
       </c>
@@ -2137,14 +2179,14 @@
       <c r="F65" s="8">
         <v>0.5</v>
       </c>
-      <c r="G65" s="38">
+      <c r="G65" s="32">
         <v>2017</v>
       </c>
-      <c r="H65" s="39">
+      <c r="H65" s="33">
         <v>93</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A66" s="7">
         <v>10</v>
       </c>
@@ -2170,7 +2212,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A67" s="7">
         <v>10</v>
       </c>
@@ -2189,14 +2231,14 @@
       <c r="F67" s="8">
         <v>0.5</v>
       </c>
-      <c r="G67" s="38">
+      <c r="G67" s="32">
         <v>1098</v>
       </c>
-      <c r="H67" s="39">
+      <c r="H67" s="33">
         <v>93</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A68" s="7">
         <v>10</v>
       </c>
@@ -2215,14 +2257,14 @@
       <c r="F68" s="8">
         <v>0.5</v>
       </c>
-      <c r="G68" s="38">
+      <c r="G68" s="32">
         <v>924</v>
       </c>
-      <c r="H68" s="39">
+      <c r="H68" s="33">
         <v>91</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A69" s="12">
         <v>10</v>
       </c>
@@ -2248,7 +2290,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A70" s="12">
         <v>10</v>
       </c>
@@ -2274,7 +2316,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A71" s="12">
         <v>10</v>
       </c>
@@ -2300,29 +2342,29 @@
         <v>94</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="40">
+    <row r="72" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A72" s="34">
         <v>10</v>
       </c>
-      <c r="B72" s="41">
+      <c r="B72" s="35">
         <v>50</v>
       </c>
-      <c r="C72" s="42">
+      <c r="C72" s="36">
         <v>180</v>
       </c>
-      <c r="D72" s="43">
-        <v>1</v>
-      </c>
-      <c r="E72" s="43">
-        <v>0</v>
-      </c>
-      <c r="F72" s="41">
-        <v>0.5</v>
-      </c>
-      <c r="G72" s="44">
+      <c r="D72" s="37">
+        <v>1</v>
+      </c>
+      <c r="E72" s="37">
+        <v>0</v>
+      </c>
+      <c r="F72" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="G72" s="38">
         <v>866</v>
       </c>
-      <c r="H72" s="45">
+      <c r="H72" s="39">
         <v>90</v>
       </c>
     </row>
@@ -2338,24 +2380,848 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8CD177C-490A-4D10-8E2D-14EA55971F52}">
+  <dimension ref="A1:J38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="3" width="18.73046875" customWidth="1"/>
+    <col min="4" max="4" width="18.73046875" style="1" customWidth="1"/>
+    <col min="5" max="6" width="18.73046875" customWidth="1"/>
+    <col min="7" max="7" width="15.73046875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.73046875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="52.73046875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A1" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="42"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A3" s="12">
+        <v>5</v>
+      </c>
+      <c r="B3" s="13">
+        <v>30</v>
+      </c>
+      <c r="C3" s="13">
+        <v>140</v>
+      </c>
+      <c r="D3" s="14">
+        <v>1</v>
+      </c>
+      <c r="E3" s="14">
+        <v>0</v>
+      </c>
+      <c r="F3" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G3" s="14"/>
+      <c r="H3" s="13"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A4" s="12">
+        <v>5</v>
+      </c>
+      <c r="B4" s="13">
+        <v>30</v>
+      </c>
+      <c r="C4" s="13">
+        <v>160</v>
+      </c>
+      <c r="D4" s="14">
+        <v>1</v>
+      </c>
+      <c r="E4" s="14">
+        <v>0</v>
+      </c>
+      <c r="F4" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="14">
+        <v>1361</v>
+      </c>
+      <c r="H4" s="13">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A5" s="12">
+        <v>5</v>
+      </c>
+      <c r="B5" s="13">
+        <v>30</v>
+      </c>
+      <c r="C5" s="16">
+        <v>180</v>
+      </c>
+      <c r="D5" s="14">
+        <v>1</v>
+      </c>
+      <c r="E5" s="14">
+        <v>0</v>
+      </c>
+      <c r="F5" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G5" s="14">
+        <v>1119</v>
+      </c>
+      <c r="H5" s="13">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A6" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" s="13">
+        <v>30</v>
+      </c>
+      <c r="C6" s="13">
+        <v>200</v>
+      </c>
+      <c r="D6" s="14">
+        <v>1</v>
+      </c>
+      <c r="E6" s="14">
+        <v>0</v>
+      </c>
+      <c r="F6" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G6" s="14"/>
+      <c r="H6" s="13"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A7" s="7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="8">
+        <v>40</v>
+      </c>
+      <c r="C7" s="8">
+        <v>140</v>
+      </c>
+      <c r="D7" s="9">
+        <v>1</v>
+      </c>
+      <c r="E7" s="9">
+        <v>0</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G7" s="9"/>
+      <c r="H7" s="8"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A8" s="7">
+        <v>5</v>
+      </c>
+      <c r="B8" s="8">
+        <v>40</v>
+      </c>
+      <c r="C8" s="8">
+        <v>160</v>
+      </c>
+      <c r="D8" s="9">
+        <v>1</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G8" s="9"/>
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A9" s="7">
+        <v>5</v>
+      </c>
+      <c r="B9" s="8">
+        <v>40</v>
+      </c>
+      <c r="C9" s="11">
+        <v>180</v>
+      </c>
+      <c r="D9" s="9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="9">
+        <v>0</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G9" s="9"/>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A10" s="7">
+        <v>5</v>
+      </c>
+      <c r="B10" s="8">
+        <v>40</v>
+      </c>
+      <c r="C10" s="8">
+        <v>200</v>
+      </c>
+      <c r="D10" s="9">
+        <v>1</v>
+      </c>
+      <c r="E10" s="9">
+        <v>0</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="9"/>
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A11" s="12">
+        <v>5</v>
+      </c>
+      <c r="B11" s="13">
+        <v>50</v>
+      </c>
+      <c r="C11" s="13">
+        <v>140</v>
+      </c>
+      <c r="D11" s="14">
+        <v>1</v>
+      </c>
+      <c r="E11" s="14">
+        <v>0</v>
+      </c>
+      <c r="F11" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G11" s="14"/>
+      <c r="H11" s="13"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A12" s="12">
+        <v>5</v>
+      </c>
+      <c r="B12" s="13">
+        <v>50</v>
+      </c>
+      <c r="C12" s="13">
+        <v>160</v>
+      </c>
+      <c r="D12" s="14">
+        <v>1</v>
+      </c>
+      <c r="E12" s="14">
+        <v>0</v>
+      </c>
+      <c r="F12" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G12" s="14"/>
+      <c r="H12" s="13"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A13" s="12">
+        <v>5</v>
+      </c>
+      <c r="B13" s="13">
+        <v>50</v>
+      </c>
+      <c r="C13" s="16">
+        <v>180</v>
+      </c>
+      <c r="D13" s="14">
+        <v>1</v>
+      </c>
+      <c r="E13" s="14">
+        <v>0</v>
+      </c>
+      <c r="F13" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G13" s="14"/>
+      <c r="H13" s="13"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A14" s="12">
+        <v>5</v>
+      </c>
+      <c r="B14" s="13">
+        <v>50</v>
+      </c>
+      <c r="C14" s="13">
+        <v>200</v>
+      </c>
+      <c r="D14" s="14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="14">
+        <v>0</v>
+      </c>
+      <c r="F14" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G14" s="14"/>
+      <c r="H14" s="13"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A15" s="7">
+        <v>5</v>
+      </c>
+      <c r="B15" s="8">
+        <v>60</v>
+      </c>
+      <c r="C15" s="8">
+        <v>140</v>
+      </c>
+      <c r="D15" s="9">
+        <v>1</v>
+      </c>
+      <c r="E15" s="9">
+        <v>0</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G15" s="9"/>
+      <c r="H15" s="10"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A16" s="7">
+        <v>5</v>
+      </c>
+      <c r="B16" s="8">
+        <v>60</v>
+      </c>
+      <c r="C16" s="8">
+        <v>160</v>
+      </c>
+      <c r="D16" s="9">
+        <v>1</v>
+      </c>
+      <c r="E16" s="9">
+        <v>0</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G16" s="9"/>
+      <c r="H16" s="10"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A17" s="7">
+        <v>5</v>
+      </c>
+      <c r="B17" s="8">
+        <v>60</v>
+      </c>
+      <c r="C17" s="11">
+        <v>180</v>
+      </c>
+      <c r="D17" s="9">
+        <v>1</v>
+      </c>
+      <c r="E17" s="9">
+        <v>0</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G17" s="9"/>
+      <c r="H17" s="10"/>
+    </row>
+    <row r="18" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="17">
+        <v>5</v>
+      </c>
+      <c r="B18" s="18">
+        <v>60</v>
+      </c>
+      <c r="C18" s="18">
+        <v>200</v>
+      </c>
+      <c r="D18" s="19">
+        <v>1</v>
+      </c>
+      <c r="E18" s="19">
+        <v>0</v>
+      </c>
+      <c r="F18" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="G18" s="19"/>
+      <c r="H18" s="20"/>
+    </row>
+    <row r="20" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A21" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="42"/>
+      <c r="J21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A22" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A23" s="12">
+        <v>10</v>
+      </c>
+      <c r="B23" s="13">
+        <v>30</v>
+      </c>
+      <c r="C23" s="13">
+        <v>140</v>
+      </c>
+      <c r="D23" s="14">
+        <v>1</v>
+      </c>
+      <c r="E23" s="14">
+        <v>0</v>
+      </c>
+      <c r="F23" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G23" s="14"/>
+      <c r="H23" s="13"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A24" s="12">
+        <v>10</v>
+      </c>
+      <c r="B24" s="13">
+        <v>30</v>
+      </c>
+      <c r="C24" s="13">
+        <v>160</v>
+      </c>
+      <c r="D24" s="14">
+        <v>1</v>
+      </c>
+      <c r="E24" s="14">
+        <v>0</v>
+      </c>
+      <c r="F24" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G24" s="14"/>
+      <c r="H24" s="13"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A25" s="12">
+        <v>10</v>
+      </c>
+      <c r="B25" s="13">
+        <v>30</v>
+      </c>
+      <c r="C25" s="16">
+        <v>180</v>
+      </c>
+      <c r="D25" s="14">
+        <v>1</v>
+      </c>
+      <c r="E25" s="14">
+        <v>0</v>
+      </c>
+      <c r="F25" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G25" s="14"/>
+      <c r="H25" s="13"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A26" s="12">
+        <v>10</v>
+      </c>
+      <c r="B26" s="13">
+        <v>30</v>
+      </c>
+      <c r="C26" s="13">
+        <v>200</v>
+      </c>
+      <c r="D26" s="14">
+        <v>1</v>
+      </c>
+      <c r="E26" s="14">
+        <v>0</v>
+      </c>
+      <c r="F26" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G26" s="14"/>
+      <c r="H26" s="13"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A27" s="7">
+        <v>10</v>
+      </c>
+      <c r="B27" s="8">
+        <v>40</v>
+      </c>
+      <c r="C27" s="8">
+        <v>140</v>
+      </c>
+      <c r="D27" s="9">
+        <v>1</v>
+      </c>
+      <c r="E27" s="9">
+        <v>0</v>
+      </c>
+      <c r="F27" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G27" s="9"/>
+      <c r="H27" s="8"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A28" s="7">
+        <v>10</v>
+      </c>
+      <c r="B28" s="8">
+        <v>40</v>
+      </c>
+      <c r="C28" s="8">
+        <v>160</v>
+      </c>
+      <c r="D28" s="9">
+        <v>1</v>
+      </c>
+      <c r="E28" s="9">
+        <v>0</v>
+      </c>
+      <c r="F28" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G28" s="9"/>
+      <c r="H28" s="8"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A29" s="7">
+        <v>10</v>
+      </c>
+      <c r="B29" s="8">
+        <v>40</v>
+      </c>
+      <c r="C29" s="11">
+        <v>180</v>
+      </c>
+      <c r="D29" s="9">
+        <v>1</v>
+      </c>
+      <c r="E29" s="9">
+        <v>0</v>
+      </c>
+      <c r="F29" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G29" s="9"/>
+      <c r="H29" s="8"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A30" s="7">
+        <v>10</v>
+      </c>
+      <c r="B30" s="8">
+        <v>40</v>
+      </c>
+      <c r="C30" s="8">
+        <v>200</v>
+      </c>
+      <c r="D30" s="9">
+        <v>1</v>
+      </c>
+      <c r="E30" s="9">
+        <v>0</v>
+      </c>
+      <c r="F30" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G30" s="9"/>
+      <c r="H30" s="8"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A31" s="12">
+        <v>10</v>
+      </c>
+      <c r="B31" s="13">
+        <v>50</v>
+      </c>
+      <c r="C31" s="13">
+        <v>140</v>
+      </c>
+      <c r="D31" s="14">
+        <v>1</v>
+      </c>
+      <c r="E31" s="14">
+        <v>0</v>
+      </c>
+      <c r="F31" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G31" s="14"/>
+      <c r="H31" s="13"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A32" s="12">
+        <v>10</v>
+      </c>
+      <c r="B32" s="13">
+        <v>50</v>
+      </c>
+      <c r="C32" s="13">
+        <v>160</v>
+      </c>
+      <c r="D32" s="14">
+        <v>1</v>
+      </c>
+      <c r="E32" s="14">
+        <v>0</v>
+      </c>
+      <c r="F32" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G32" s="14"/>
+      <c r="H32" s="13"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A33" s="12">
+        <v>10</v>
+      </c>
+      <c r="B33" s="13">
+        <v>50</v>
+      </c>
+      <c r="C33" s="16">
+        <v>180</v>
+      </c>
+      <c r="D33" s="14">
+        <v>1</v>
+      </c>
+      <c r="E33" s="14">
+        <v>0</v>
+      </c>
+      <c r="F33" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G33" s="14"/>
+      <c r="H33" s="13"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A34" s="12">
+        <v>10</v>
+      </c>
+      <c r="B34" s="13">
+        <v>50</v>
+      </c>
+      <c r="C34" s="13">
+        <v>200</v>
+      </c>
+      <c r="D34" s="14">
+        <v>1</v>
+      </c>
+      <c r="E34" s="14">
+        <v>0</v>
+      </c>
+      <c r="F34" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G34" s="14"/>
+      <c r="H34" s="13"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A35" s="7">
+        <v>10</v>
+      </c>
+      <c r="B35" s="8">
+        <v>60</v>
+      </c>
+      <c r="C35" s="8">
+        <v>140</v>
+      </c>
+      <c r="D35" s="9">
+        <v>1</v>
+      </c>
+      <c r="E35" s="9">
+        <v>0</v>
+      </c>
+      <c r="F35" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G35" s="9"/>
+      <c r="H35" s="10"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A36" s="7">
+        <v>10</v>
+      </c>
+      <c r="B36" s="8">
+        <v>60</v>
+      </c>
+      <c r="C36" s="8">
+        <v>160</v>
+      </c>
+      <c r="D36" s="9">
+        <v>1</v>
+      </c>
+      <c r="E36" s="9">
+        <v>0</v>
+      </c>
+      <c r="F36" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G36" s="9"/>
+      <c r="H36" s="10"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A37" s="7">
+        <v>10</v>
+      </c>
+      <c r="B37" s="8">
+        <v>60</v>
+      </c>
+      <c r="C37" s="11">
+        <v>180</v>
+      </c>
+      <c r="D37" s="9">
+        <v>1</v>
+      </c>
+      <c r="E37" s="9">
+        <v>0</v>
+      </c>
+      <c r="F37" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G37" s="9"/>
+      <c r="H37" s="10"/>
+    </row>
+    <row r="38" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A38" s="7">
+        <v>10</v>
+      </c>
+      <c r="B38" s="18">
+        <v>60</v>
+      </c>
+      <c r="C38" s="18">
+        <v>200</v>
+      </c>
+      <c r="D38" s="19">
+        <v>1</v>
+      </c>
+      <c r="E38" s="19">
+        <v>0</v>
+      </c>
+      <c r="F38" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="G38" s="19"/>
+      <c r="H38" s="20"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A21:H21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updating the validation set points again
</commit_message>
<xml_diff>
--- a/GHT/validation_set_results.xlsx
+++ b/GHT/validation_set_results.xlsx
@@ -3,15 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE93E26-6F72-4046-9930-727D4CC40B53}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632024F7-CA8E-43DE-BD63-C12CA574E805}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Interim Report" sheetId="1" r:id="rId1"/>
     <sheet name="Power 6 Prior + Top 5 Avg" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -2384,7 +2382,7 @@
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3201,28 +3199,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Modified to work with final testing
</commit_message>
<xml_diff>
--- a/GHT/validation_set_results.xlsx
+++ b/GHT/validation_set_results.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632024F7-CA8E-43DE-BD63-C12CA574E805}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Interim Report" sheetId="1" r:id="rId1"/>
-    <sheet name="Power 6 Prior + Top 5 Avg" sheetId="4" r:id="rId2"/>
+    <sheet name="Power 4 Prior + Top 5 Avg" sheetId="4" r:id="rId2"/>
+    <sheet name="No Prior + Top 5 Avg" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="15">
   <si>
     <t>Min Canny</t>
   </si>
@@ -57,13 +59,16 @@
     <t>First 5 References (7796800, 6268647, 9049401, 6729799, 8476267)</t>
   </si>
   <si>
-    <t>Validation Set Result for C1 Spine Detection: Power 6 Prior + Top 5 Avg</t>
+    <t>Validation Set Result for C1 Spine Detection: Power 4 Prior + Top 5 Avg</t>
+  </si>
+  <si>
+    <t>Validation Set Result for C1 Spine Detection: No Prior + Top 5 Avg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -294,7 +299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -363,6 +368,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,7 +437,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -456,26 +470,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -508,23 +505,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -700,25 +680,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="3" width="18.73046875" customWidth="1"/>
-    <col min="4" max="4" width="18.73046875" style="1" customWidth="1"/>
-    <col min="5" max="6" width="18.73046875" customWidth="1"/>
-    <col min="7" max="7" width="15.73046875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.73046875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="52.73046875" customWidth="1"/>
+    <col min="2" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="1" customWidth="1"/>
+    <col min="5" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="52.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A1" s="40" t="s">
         <v>6</v>
       </c>
@@ -730,7 +710,7 @@
       <c r="G1" s="41"/>
       <c r="H1" s="42"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
@@ -759,7 +739,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" s="7">
         <v>5</v>
       </c>
@@ -788,7 +768,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" s="7">
         <v>5</v>
       </c>
@@ -817,7 +797,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" s="7">
         <v>5</v>
       </c>
@@ -843,7 +823,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -869,7 +849,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -895,7 +875,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A8" s="12">
         <v>5</v>
       </c>
@@ -921,7 +901,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A9" s="12">
         <v>5</v>
       </c>
@@ -947,7 +927,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A10" s="12">
         <v>5</v>
       </c>
@@ -973,7 +953,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A11" s="12">
         <v>5</v>
       </c>
@@ -999,7 +979,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A12" s="12">
         <v>5</v>
       </c>
@@ -1025,7 +1005,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A13" s="7">
         <v>5</v>
       </c>
@@ -1051,7 +1031,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A14" s="7">
         <v>5</v>
       </c>
@@ -1077,7 +1057,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A15" s="7">
         <v>5</v>
       </c>
@@ -1103,7 +1083,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A16" s="7">
         <v>5</v>
       </c>
@@ -1129,7 +1109,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A17" s="7">
         <v>5</v>
       </c>
@@ -1155,7 +1135,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A18" s="12">
         <v>5</v>
       </c>
@@ -1181,7 +1161,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A19" s="12">
         <v>5</v>
       </c>
@@ -1207,7 +1187,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A20" s="12">
         <v>5</v>
       </c>
@@ -1233,7 +1213,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A21" s="12">
         <v>5</v>
       </c>
@@ -1255,7 +1235,7 @@
       <c r="G21" s="14"/>
       <c r="H21" s="15"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A22" s="12">
         <v>5</v>
       </c>
@@ -1277,7 +1257,7 @@
       <c r="G22" s="14"/>
       <c r="H22" s="15"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A23" s="7">
         <v>5</v>
       </c>
@@ -1299,7 +1279,7 @@
       <c r="G23" s="9"/>
       <c r="H23" s="10"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A24" s="7">
         <v>5</v>
       </c>
@@ -1321,7 +1301,7 @@
       <c r="G24" s="9"/>
       <c r="H24" s="10"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A25" s="7">
         <v>5</v>
       </c>
@@ -1343,7 +1323,7 @@
       <c r="G25" s="9"/>
       <c r="H25" s="10"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A26" s="7">
         <v>5</v>
       </c>
@@ -1388,7 +1368,7 @@
       <c r="H27" s="20"/>
     </row>
     <row r="29" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A30" s="43" t="s">
         <v>6</v>
       </c>
@@ -1403,7 +1383,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A31" s="5" t="s">
         <v>8</v>
       </c>
@@ -1429,7 +1409,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A32" s="7">
         <v>1</v>
       </c>
@@ -1455,7 +1435,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A33" s="7">
         <v>1</v>
       </c>
@@ -1481,7 +1461,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A34" s="7">
         <v>1</v>
       </c>
@@ -1507,7 +1487,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A35" s="7">
         <v>1</v>
       </c>
@@ -1533,7 +1513,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A36" s="7">
         <v>1</v>
       </c>
@@ -1559,7 +1539,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A37" s="12">
         <v>1</v>
       </c>
@@ -1585,7 +1565,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A38" s="12">
         <v>1</v>
       </c>
@@ -1611,7 +1591,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A39" s="12">
         <v>1</v>
       </c>
@@ -1637,7 +1617,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A40" s="12">
         <v>1</v>
       </c>
@@ -1663,7 +1643,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A41" s="12">
         <v>1</v>
       </c>
@@ -1685,7 +1665,7 @@
       <c r="G41" s="14"/>
       <c r="H41" s="15"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A42" s="7">
         <v>1</v>
       </c>
@@ -1707,7 +1687,7 @@
       <c r="G42" s="9"/>
       <c r="H42" s="10"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <v>1</v>
       </c>
@@ -1729,7 +1709,7 @@
       <c r="G43" s="9"/>
       <c r="H43" s="10"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
         <v>1</v>
       </c>
@@ -1751,7 +1731,7 @@
       <c r="G44" s="9"/>
       <c r="H44" s="10"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
         <v>1</v>
       </c>
@@ -1773,7 +1753,7 @@
       <c r="G45" s="9"/>
       <c r="H45" s="10"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
         <v>1</v>
       </c>
@@ -1795,7 +1775,7 @@
       <c r="G46" s="9"/>
       <c r="H46" s="10"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="12">
         <v>1</v>
       </c>
@@ -1817,7 +1797,7 @@
       <c r="G47" s="14"/>
       <c r="H47" s="15"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="12">
         <v>1</v>
       </c>
@@ -1839,7 +1819,7 @@
       <c r="G48" s="14"/>
       <c r="H48" s="15"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="12">
         <v>1</v>
       </c>
@@ -1861,7 +1841,7 @@
       <c r="G49" s="14"/>
       <c r="H49" s="15"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="12">
         <v>1</v>
       </c>
@@ -1883,7 +1863,7 @@
       <c r="G50" s="14"/>
       <c r="H50" s="15"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="12">
         <v>1</v>
       </c>
@@ -1905,7 +1885,7 @@
       <c r="G51" s="14"/>
       <c r="H51" s="15"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="7">
         <v>1</v>
       </c>
@@ -1927,7 +1907,7 @@
       <c r="G52" s="9"/>
       <c r="H52" s="10"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="7">
         <v>1</v>
       </c>
@@ -1949,7 +1929,7 @@
       <c r="G53" s="9"/>
       <c r="H53" s="10"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
         <v>1</v>
       </c>
@@ -1971,7 +1951,7 @@
       <c r="G54" s="9"/>
       <c r="H54" s="10"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="7">
         <v>1</v>
       </c>
@@ -1993,7 +1973,7 @@
       <c r="G55" s="9"/>
       <c r="H55" s="10"/>
     </row>
-    <row r="56" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="7">
         <v>1</v>
       </c>
@@ -2015,8 +1995,8 @@
       <c r="G56" s="19"/>
       <c r="H56" s="20"/>
     </row>
-    <row r="58" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="40" t="s">
         <v>6</v>
       </c>
@@ -2028,7 +2008,7 @@
       <c r="G59" s="41"/>
       <c r="H59" s="42"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>8</v>
       </c>
@@ -2054,7 +2034,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="12">
         <v>10</v>
       </c>
@@ -2080,7 +2060,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="12">
         <v>10</v>
       </c>
@@ -2106,7 +2086,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="12">
         <v>10</v>
       </c>
@@ -2132,7 +2112,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="12">
         <v>10</v>
       </c>
@@ -2158,7 +2138,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="7">
         <v>10</v>
       </c>
@@ -2184,7 +2164,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="7">
         <v>10</v>
       </c>
@@ -2210,7 +2190,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="7">
         <v>10</v>
       </c>
@@ -2236,7 +2216,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="7">
         <v>10</v>
       </c>
@@ -2262,7 +2242,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="12">
         <v>10</v>
       </c>
@@ -2288,7 +2268,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="12">
         <v>10</v>
       </c>
@@ -2314,7 +2294,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="12">
         <v>10</v>
       </c>
@@ -2340,7 +2320,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="34">
         <v>10</v>
       </c>
@@ -2378,25 +2358,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8CD177C-490A-4D10-8E2D-14EA55971F52}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="3" width="18.73046875" customWidth="1"/>
-    <col min="4" max="4" width="18.73046875" style="1" customWidth="1"/>
-    <col min="5" max="6" width="18.73046875" customWidth="1"/>
-    <col min="7" max="7" width="15.73046875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.73046875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="52.73046875" customWidth="1"/>
+    <col min="2" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="1" customWidth="1"/>
+    <col min="5" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="52.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A1" s="40" t="s">
         <v>13</v>
       </c>
@@ -2408,7 +2388,7 @@
       <c r="G1" s="41"/>
       <c r="H1" s="42"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
@@ -2437,14 +2417,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>5</v>
       </c>
       <c r="B3" s="13">
         <v>30</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="24">
         <v>140</v>
       </c>
       <c r="D3" s="14">
@@ -2456,17 +2436,21 @@
       <c r="F3" s="13">
         <v>0.5</v>
       </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="13"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="G3" s="14">
+        <v>1071</v>
+      </c>
+      <c r="H3" s="53">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>5</v>
       </c>
       <c r="B4" s="13">
         <v>30</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="24">
         <v>160</v>
       </c>
       <c r="D4" s="14">
@@ -2479,20 +2463,20 @@
         <v>0.5</v>
       </c>
       <c r="G4" s="14">
-        <v>1361</v>
-      </c>
-      <c r="H4" s="13">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+        <v>1327</v>
+      </c>
+      <c r="H4" s="53">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>5</v>
       </c>
       <c r="B5" s="13">
         <v>30</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="24">
         <v>180</v>
       </c>
       <c r="D5" s="14">
@@ -2505,20 +2489,20 @@
         <v>0.5</v>
       </c>
       <c r="G5" s="14">
-        <v>1119</v>
-      </c>
-      <c r="H5" s="13">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+        <v>1198</v>
+      </c>
+      <c r="H5" s="53">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>5</v>
       </c>
       <c r="B6" s="13">
         <v>30</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="24">
         <v>200</v>
       </c>
       <c r="D6" s="14">
@@ -2530,17 +2514,21 @@
       <c r="F6" s="13">
         <v>0.5</v>
       </c>
-      <c r="G6" s="14"/>
-      <c r="H6" s="13"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="G6" s="14">
+        <v>1369</v>
+      </c>
+      <c r="H6" s="53">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>5</v>
       </c>
       <c r="B7" s="8">
         <v>40</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="23">
         <v>140</v>
       </c>
       <c r="D7" s="9">
@@ -2552,17 +2540,21 @@
       <c r="F7" s="8">
         <v>0.5</v>
       </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="8"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="G7" s="9">
+        <v>979</v>
+      </c>
+      <c r="H7" s="54">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>5</v>
       </c>
       <c r="B8" s="8">
         <v>40</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="23">
         <v>160</v>
       </c>
       <c r="D8" s="9">
@@ -2574,17 +2566,21 @@
       <c r="F8" s="8">
         <v>0.5</v>
       </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="8"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="G8" s="9">
+        <v>1120</v>
+      </c>
+      <c r="H8" s="54">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>5</v>
       </c>
       <c r="B9" s="8">
         <v>40</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="23">
         <v>180</v>
       </c>
       <c r="D9" s="9">
@@ -2596,17 +2592,21 @@
       <c r="F9" s="8">
         <v>0.5</v>
       </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="8"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="G9" s="9">
+        <v>1049</v>
+      </c>
+      <c r="H9" s="54">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>5</v>
       </c>
       <c r="B10" s="8">
         <v>40</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="23">
         <v>200</v>
       </c>
       <c r="D10" s="9">
@@ -2618,17 +2618,21 @@
       <c r="F10" s="8">
         <v>0.5</v>
       </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="8"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="G10" s="9">
+        <v>1265</v>
+      </c>
+      <c r="H10" s="54">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>5</v>
       </c>
       <c r="B11" s="13">
         <v>50</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="24">
         <v>140</v>
       </c>
       <c r="D11" s="14">
@@ -2641,16 +2645,16 @@
         <v>0.5</v>
       </c>
       <c r="G11" s="14"/>
-      <c r="H11" s="13"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="H11" s="53"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>5</v>
       </c>
       <c r="B12" s="13">
         <v>50</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="24">
         <v>160</v>
       </c>
       <c r="D12" s="14">
@@ -2663,16 +2667,16 @@
         <v>0.5</v>
       </c>
       <c r="G12" s="14"/>
-      <c r="H12" s="13"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="H12" s="53"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>5</v>
       </c>
       <c r="B13" s="13">
         <v>50</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13" s="24">
         <v>180</v>
       </c>
       <c r="D13" s="14">
@@ -2685,16 +2689,16 @@
         <v>0.5</v>
       </c>
       <c r="G13" s="14"/>
-      <c r="H13" s="13"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="H13" s="53"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>5</v>
       </c>
       <c r="B14" s="13">
         <v>50</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="24">
         <v>200</v>
       </c>
       <c r="D14" s="14">
@@ -2707,16 +2711,16 @@
         <v>0.5</v>
       </c>
       <c r="G14" s="14"/>
-      <c r="H14" s="13"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="H14" s="53"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>5</v>
       </c>
       <c r="B15" s="8">
         <v>60</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="23">
         <v>140</v>
       </c>
       <c r="D15" s="9">
@@ -2731,14 +2735,14 @@
       <c r="G15" s="9"/>
       <c r="H15" s="10"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>5</v>
       </c>
       <c r="B16" s="8">
         <v>60</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="23">
         <v>160</v>
       </c>
       <c r="D16" s="9">
@@ -2753,14 +2757,14 @@
       <c r="G16" s="9"/>
       <c r="H16" s="10"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>5</v>
       </c>
       <c r="B17" s="8">
         <v>60</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="23">
         <v>180</v>
       </c>
       <c r="D17" s="9">
@@ -2775,14 +2779,14 @@
       <c r="G17" s="9"/>
       <c r="H17" s="10"/>
     </row>
-    <row r="18" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="17">
         <v>5</v>
       </c>
       <c r="B18" s="18">
         <v>60</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C18" s="25">
         <v>200</v>
       </c>
       <c r="D18" s="19">
@@ -2797,8 +2801,8 @@
       <c r="G18" s="19"/>
       <c r="H18" s="20"/>
     </row>
-    <row r="20" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="40" t="s">
         <v>6</v>
       </c>
@@ -2809,11 +2813,8 @@
       <c r="F21" s="41"/>
       <c r="G21" s="41"/>
       <c r="H21" s="42"/>
-      <c r="J21" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>8</v>
       </c>
@@ -2839,7 +2840,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>10</v>
       </c>
@@ -2859,9 +2860,9 @@
         <v>0.5</v>
       </c>
       <c r="G23" s="14"/>
-      <c r="H23" s="13"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="H23" s="53"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>10</v>
       </c>
@@ -2881,19 +2882,19 @@
         <v>0.5</v>
       </c>
       <c r="G24" s="14"/>
-      <c r="H24" s="13"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="H24" s="53"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>10</v>
       </c>
-      <c r="B25" s="13">
+      <c r="B25" s="24">
         <v>30</v>
       </c>
-      <c r="C25" s="16">
+      <c r="C25" s="24">
         <v>180</v>
       </c>
-      <c r="D25" s="14">
+      <c r="D25" s="30">
         <v>1</v>
       </c>
       <c r="E25" s="14">
@@ -2903,19 +2904,19 @@
         <v>0.5</v>
       </c>
       <c r="G25" s="14"/>
-      <c r="H25" s="13"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="H25" s="53"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>10</v>
       </c>
-      <c r="B26" s="13">
+      <c r="B26" s="24">
         <v>30</v>
       </c>
-      <c r="C26" s="13">
+      <c r="C26" s="24">
         <v>200</v>
       </c>
-      <c r="D26" s="14">
+      <c r="D26" s="30">
         <v>1</v>
       </c>
       <c r="E26" s="14">
@@ -2925,19 +2926,19 @@
         <v>0.5</v>
       </c>
       <c r="G26" s="14"/>
-      <c r="H26" s="13"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="H26" s="53"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>10</v>
       </c>
-      <c r="B27" s="8">
+      <c r="B27" s="23">
         <v>40</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C27" s="23">
         <v>140</v>
       </c>
-      <c r="D27" s="9">
+      <c r="D27" s="32">
         <v>1</v>
       </c>
       <c r="E27" s="9">
@@ -2947,19 +2948,19 @@
         <v>0.5</v>
       </c>
       <c r="G27" s="9"/>
-      <c r="H27" s="8"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="H27" s="54"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <v>10</v>
       </c>
-      <c r="B28" s="8">
+      <c r="B28" s="23">
         <v>40</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C28" s="23">
         <v>160</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D28" s="32">
         <v>1</v>
       </c>
       <c r="E28" s="9">
@@ -2969,19 +2970,19 @@
         <v>0.5</v>
       </c>
       <c r="G28" s="9"/>
-      <c r="H28" s="8"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="H28" s="54"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>10</v>
       </c>
-      <c r="B29" s="8">
+      <c r="B29" s="23">
         <v>40</v>
       </c>
-      <c r="C29" s="11">
+      <c r="C29" s="23">
         <v>180</v>
       </c>
-      <c r="D29" s="9">
+      <c r="D29" s="32">
         <v>1</v>
       </c>
       <c r="E29" s="9">
@@ -2991,19 +2992,19 @@
         <v>0.5</v>
       </c>
       <c r="G29" s="9"/>
-      <c r="H29" s="8"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="H29" s="54"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <v>10</v>
       </c>
-      <c r="B30" s="8">
+      <c r="B30" s="23">
         <v>40</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="23">
         <v>200</v>
       </c>
-      <c r="D30" s="9">
+      <c r="D30" s="32">
         <v>1</v>
       </c>
       <c r="E30" s="9">
@@ -3013,19 +3014,19 @@
         <v>0.5</v>
       </c>
       <c r="G30" s="9"/>
-      <c r="H30" s="8"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="H30" s="54"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <v>10</v>
       </c>
-      <c r="B31" s="13">
+      <c r="B31" s="24">
         <v>50</v>
       </c>
-      <c r="C31" s="13">
+      <c r="C31" s="24">
         <v>140</v>
       </c>
-      <c r="D31" s="14">
+      <c r="D31" s="30">
         <v>1</v>
       </c>
       <c r="E31" s="14">
@@ -3035,19 +3036,19 @@
         <v>0.5</v>
       </c>
       <c r="G31" s="14"/>
-      <c r="H31" s="13"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="H31" s="53"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>10</v>
       </c>
-      <c r="B32" s="13">
+      <c r="B32" s="24">
         <v>50</v>
       </c>
-      <c r="C32" s="13">
+      <c r="C32" s="24">
         <v>160</v>
       </c>
-      <c r="D32" s="14">
+      <c r="D32" s="30">
         <v>1</v>
       </c>
       <c r="E32" s="14">
@@ -3057,19 +3058,19 @@
         <v>0.5</v>
       </c>
       <c r="G32" s="14"/>
-      <c r="H32" s="13"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="H32" s="53"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <v>10</v>
       </c>
-      <c r="B33" s="13">
+      <c r="B33" s="24">
         <v>50</v>
       </c>
-      <c r="C33" s="16">
+      <c r="C33" s="24">
         <v>180</v>
       </c>
-      <c r="D33" s="14">
+      <c r="D33" s="30">
         <v>1</v>
       </c>
       <c r="E33" s="14">
@@ -3079,19 +3080,19 @@
         <v>0.5</v>
       </c>
       <c r="G33" s="14"/>
-      <c r="H33" s="13"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="H33" s="53"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <v>10</v>
       </c>
-      <c r="B34" s="13">
+      <c r="B34" s="24">
         <v>50</v>
       </c>
-      <c r="C34" s="13">
+      <c r="C34" s="24">
         <v>200</v>
       </c>
-      <c r="D34" s="14">
+      <c r="D34" s="30">
         <v>1</v>
       </c>
       <c r="E34" s="14">
@@ -3101,19 +3102,19 @@
         <v>0.5</v>
       </c>
       <c r="G34" s="14"/>
-      <c r="H34" s="13"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="H34" s="53"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>10</v>
       </c>
-      <c r="B35" s="8">
+      <c r="B35" s="23">
         <v>60</v>
       </c>
-      <c r="C35" s="8">
+      <c r="C35" s="23">
         <v>140</v>
       </c>
-      <c r="D35" s="9">
+      <c r="D35" s="32">
         <v>1</v>
       </c>
       <c r="E35" s="9">
@@ -3125,17 +3126,17 @@
       <c r="G35" s="9"/>
       <c r="H35" s="10"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <v>10</v>
       </c>
-      <c r="B36" s="8">
+      <c r="B36" s="23">
         <v>60</v>
       </c>
-      <c r="C36" s="8">
+      <c r="C36" s="23">
         <v>160</v>
       </c>
-      <c r="D36" s="9">
+      <c r="D36" s="32">
         <v>1</v>
       </c>
       <c r="E36" s="9">
@@ -3147,17 +3148,17 @@
       <c r="G36" s="9"/>
       <c r="H36" s="10"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>10</v>
       </c>
-      <c r="B37" s="8">
+      <c r="B37" s="23">
         <v>60</v>
       </c>
-      <c r="C37" s="11">
+      <c r="C37" s="23">
         <v>180</v>
       </c>
-      <c r="D37" s="9">
+      <c r="D37" s="32">
         <v>1</v>
       </c>
       <c r="E37" s="9">
@@ -3169,17 +3170,17 @@
       <c r="G37" s="9"/>
       <c r="H37" s="10"/>
     </row>
-    <row r="38" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A38" s="7">
-        <v>10</v>
-      </c>
-      <c r="B38" s="18">
+    <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="17">
+        <v>10</v>
+      </c>
+      <c r="B38" s="25">
         <v>60</v>
       </c>
-      <c r="C38" s="18">
+      <c r="C38" s="25">
         <v>200</v>
       </c>
-      <c r="D38" s="19">
+      <c r="D38" s="48">
         <v>1</v>
       </c>
       <c r="E38" s="19">
@@ -3199,4 +3200,849 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="1" customWidth="1"/>
+    <col min="5" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="52.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="42"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
+        <v>5</v>
+      </c>
+      <c r="B3" s="13">
+        <v>30</v>
+      </c>
+      <c r="C3" s="24">
+        <v>140</v>
+      </c>
+      <c r="D3" s="14">
+        <v>1</v>
+      </c>
+      <c r="E3" s="14">
+        <v>0</v>
+      </c>
+      <c r="F3" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G3" s="14">
+        <v>891</v>
+      </c>
+      <c r="H3" s="53">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>5</v>
+      </c>
+      <c r="B4" s="13">
+        <v>30</v>
+      </c>
+      <c r="C4" s="24">
+        <v>160</v>
+      </c>
+      <c r="D4" s="14">
+        <v>1</v>
+      </c>
+      <c r="E4" s="14">
+        <v>0</v>
+      </c>
+      <c r="F4" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="14">
+        <v>1120</v>
+      </c>
+      <c r="H4" s="53">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>5</v>
+      </c>
+      <c r="B5" s="13">
+        <v>30</v>
+      </c>
+      <c r="C5" s="24">
+        <v>180</v>
+      </c>
+      <c r="D5" s="14">
+        <v>1</v>
+      </c>
+      <c r="E5" s="14">
+        <v>0</v>
+      </c>
+      <c r="F5" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G5" s="14"/>
+      <c r="H5" s="53"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" s="13">
+        <v>30</v>
+      </c>
+      <c r="C6" s="24">
+        <v>200</v>
+      </c>
+      <c r="D6" s="14">
+        <v>1</v>
+      </c>
+      <c r="E6" s="14">
+        <v>0</v>
+      </c>
+      <c r="F6" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G6" s="14"/>
+      <c r="H6" s="53"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="8">
+        <v>40</v>
+      </c>
+      <c r="C7" s="23">
+        <v>140</v>
+      </c>
+      <c r="D7" s="9">
+        <v>1</v>
+      </c>
+      <c r="E7" s="9">
+        <v>0</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G7" s="9"/>
+      <c r="H7" s="54"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>5</v>
+      </c>
+      <c r="B8" s="8">
+        <v>40</v>
+      </c>
+      <c r="C8" s="23">
+        <v>160</v>
+      </c>
+      <c r="D8" s="9">
+        <v>1</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G8" s="9"/>
+      <c r="H8" s="54"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>5</v>
+      </c>
+      <c r="B9" s="8">
+        <v>40</v>
+      </c>
+      <c r="C9" s="23">
+        <v>180</v>
+      </c>
+      <c r="D9" s="9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="9">
+        <v>0</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G9" s="9"/>
+      <c r="H9" s="54"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>5</v>
+      </c>
+      <c r="B10" s="8">
+        <v>40</v>
+      </c>
+      <c r="C10" s="23">
+        <v>200</v>
+      </c>
+      <c r="D10" s="9">
+        <v>1</v>
+      </c>
+      <c r="E10" s="9">
+        <v>0</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="9"/>
+      <c r="H10" s="54"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>5</v>
+      </c>
+      <c r="B11" s="13">
+        <v>50</v>
+      </c>
+      <c r="C11" s="24">
+        <v>140</v>
+      </c>
+      <c r="D11" s="14">
+        <v>1</v>
+      </c>
+      <c r="E11" s="14">
+        <v>0</v>
+      </c>
+      <c r="F11" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G11" s="14"/>
+      <c r="H11" s="53"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>5</v>
+      </c>
+      <c r="B12" s="13">
+        <v>50</v>
+      </c>
+      <c r="C12" s="24">
+        <v>160</v>
+      </c>
+      <c r="D12" s="14">
+        <v>1</v>
+      </c>
+      <c r="E12" s="14">
+        <v>0</v>
+      </c>
+      <c r="F12" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G12" s="14"/>
+      <c r="H12" s="53"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>5</v>
+      </c>
+      <c r="B13" s="13">
+        <v>50</v>
+      </c>
+      <c r="C13" s="24">
+        <v>180</v>
+      </c>
+      <c r="D13" s="14">
+        <v>1</v>
+      </c>
+      <c r="E13" s="14">
+        <v>0</v>
+      </c>
+      <c r="F13" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G13" s="14"/>
+      <c r="H13" s="53"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>5</v>
+      </c>
+      <c r="B14" s="13">
+        <v>50</v>
+      </c>
+      <c r="C14" s="24">
+        <v>200</v>
+      </c>
+      <c r="D14" s="14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="14">
+        <v>0</v>
+      </c>
+      <c r="F14" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G14" s="14"/>
+      <c r="H14" s="53"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>5</v>
+      </c>
+      <c r="B15" s="8">
+        <v>60</v>
+      </c>
+      <c r="C15" s="23">
+        <v>140</v>
+      </c>
+      <c r="D15" s="9">
+        <v>1</v>
+      </c>
+      <c r="E15" s="9">
+        <v>0</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G15" s="9"/>
+      <c r="H15" s="10"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>5</v>
+      </c>
+      <c r="B16" s="8">
+        <v>60</v>
+      </c>
+      <c r="C16" s="23">
+        <v>160</v>
+      </c>
+      <c r="D16" s="9">
+        <v>1</v>
+      </c>
+      <c r="E16" s="9">
+        <v>0</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G16" s="9"/>
+      <c r="H16" s="10"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>5</v>
+      </c>
+      <c r="B17" s="8">
+        <v>60</v>
+      </c>
+      <c r="C17" s="23">
+        <v>180</v>
+      </c>
+      <c r="D17" s="9">
+        <v>1</v>
+      </c>
+      <c r="E17" s="9">
+        <v>0</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G17" s="9"/>
+      <c r="H17" s="10"/>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="17">
+        <v>5</v>
+      </c>
+      <c r="B18" s="18">
+        <v>60</v>
+      </c>
+      <c r="C18" s="25">
+        <v>200</v>
+      </c>
+      <c r="D18" s="19">
+        <v>1</v>
+      </c>
+      <c r="E18" s="19">
+        <v>0</v>
+      </c>
+      <c r="F18" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="G18" s="19"/>
+      <c r="H18" s="20"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="42"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="46">
+        <v>10</v>
+      </c>
+      <c r="B23" s="24">
+        <v>30</v>
+      </c>
+      <c r="C23" s="24">
+        <v>140</v>
+      </c>
+      <c r="D23" s="30">
+        <v>1</v>
+      </c>
+      <c r="E23" s="30">
+        <v>0</v>
+      </c>
+      <c r="F23" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G23" s="30"/>
+      <c r="H23" s="50"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="46">
+        <v>10</v>
+      </c>
+      <c r="B24" s="24">
+        <v>30</v>
+      </c>
+      <c r="C24" s="24">
+        <v>160</v>
+      </c>
+      <c r="D24" s="30">
+        <v>1</v>
+      </c>
+      <c r="E24" s="30">
+        <v>0</v>
+      </c>
+      <c r="F24" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G24" s="30"/>
+      <c r="H24" s="50"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="46">
+        <v>10</v>
+      </c>
+      <c r="B25" s="24">
+        <v>30</v>
+      </c>
+      <c r="C25" s="24">
+        <v>180</v>
+      </c>
+      <c r="D25" s="30">
+        <v>1</v>
+      </c>
+      <c r="E25" s="30">
+        <v>0</v>
+      </c>
+      <c r="F25" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G25" s="30"/>
+      <c r="H25" s="50"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="46">
+        <v>10</v>
+      </c>
+      <c r="B26" s="24">
+        <v>30</v>
+      </c>
+      <c r="C26" s="24">
+        <v>200</v>
+      </c>
+      <c r="D26" s="30">
+        <v>1</v>
+      </c>
+      <c r="E26" s="30">
+        <v>0</v>
+      </c>
+      <c r="F26" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G26" s="30"/>
+      <c r="H26" s="50"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="47">
+        <v>10</v>
+      </c>
+      <c r="B27" s="23">
+        <v>40</v>
+      </c>
+      <c r="C27" s="23">
+        <v>140</v>
+      </c>
+      <c r="D27" s="32">
+        <v>1</v>
+      </c>
+      <c r="E27" s="32">
+        <v>0</v>
+      </c>
+      <c r="F27" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="G27" s="32"/>
+      <c r="H27" s="51"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="47">
+        <v>10</v>
+      </c>
+      <c r="B28" s="23">
+        <v>40</v>
+      </c>
+      <c r="C28" s="23">
+        <v>160</v>
+      </c>
+      <c r="D28" s="32">
+        <v>1</v>
+      </c>
+      <c r="E28" s="32">
+        <v>0</v>
+      </c>
+      <c r="F28" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="G28" s="32"/>
+      <c r="H28" s="51"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="47">
+        <v>10</v>
+      </c>
+      <c r="B29" s="23">
+        <v>40</v>
+      </c>
+      <c r="C29" s="23">
+        <v>180</v>
+      </c>
+      <c r="D29" s="32">
+        <v>1</v>
+      </c>
+      <c r="E29" s="32">
+        <v>0</v>
+      </c>
+      <c r="F29" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="G29" s="32"/>
+      <c r="H29" s="51"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="47">
+        <v>10</v>
+      </c>
+      <c r="B30" s="23">
+        <v>40</v>
+      </c>
+      <c r="C30" s="23">
+        <v>200</v>
+      </c>
+      <c r="D30" s="32">
+        <v>1</v>
+      </c>
+      <c r="E30" s="32">
+        <v>0</v>
+      </c>
+      <c r="F30" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="G30" s="32"/>
+      <c r="H30" s="51"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="46">
+        <v>10</v>
+      </c>
+      <c r="B31" s="24">
+        <v>50</v>
+      </c>
+      <c r="C31" s="24">
+        <v>140</v>
+      </c>
+      <c r="D31" s="30">
+        <v>1</v>
+      </c>
+      <c r="E31" s="30">
+        <v>0</v>
+      </c>
+      <c r="F31" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G31" s="30"/>
+      <c r="H31" s="50"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="46">
+        <v>10</v>
+      </c>
+      <c r="B32" s="24">
+        <v>50</v>
+      </c>
+      <c r="C32" s="24">
+        <v>160</v>
+      </c>
+      <c r="D32" s="30">
+        <v>1</v>
+      </c>
+      <c r="E32" s="30">
+        <v>0</v>
+      </c>
+      <c r="F32" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G32" s="30"/>
+      <c r="H32" s="50"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="46">
+        <v>10</v>
+      </c>
+      <c r="B33" s="24">
+        <v>50</v>
+      </c>
+      <c r="C33" s="24">
+        <v>180</v>
+      </c>
+      <c r="D33" s="30">
+        <v>1</v>
+      </c>
+      <c r="E33" s="30">
+        <v>0</v>
+      </c>
+      <c r="F33" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G33" s="30"/>
+      <c r="H33" s="50"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="46">
+        <v>10</v>
+      </c>
+      <c r="B34" s="24">
+        <v>50</v>
+      </c>
+      <c r="C34" s="24">
+        <v>200</v>
+      </c>
+      <c r="D34" s="30">
+        <v>1</v>
+      </c>
+      <c r="E34" s="30">
+        <v>0</v>
+      </c>
+      <c r="F34" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G34" s="30"/>
+      <c r="H34" s="50"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="47">
+        <v>10</v>
+      </c>
+      <c r="B35" s="23">
+        <v>60</v>
+      </c>
+      <c r="C35" s="23">
+        <v>140</v>
+      </c>
+      <c r="D35" s="32">
+        <v>1</v>
+      </c>
+      <c r="E35" s="32">
+        <v>0</v>
+      </c>
+      <c r="F35" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="G35" s="32"/>
+      <c r="H35" s="33"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="47">
+        <v>10</v>
+      </c>
+      <c r="B36" s="23">
+        <v>60</v>
+      </c>
+      <c r="C36" s="23">
+        <v>160</v>
+      </c>
+      <c r="D36" s="32">
+        <v>1</v>
+      </c>
+      <c r="E36" s="32">
+        <v>0</v>
+      </c>
+      <c r="F36" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="G36" s="32"/>
+      <c r="H36" s="33"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="47">
+        <v>10</v>
+      </c>
+      <c r="B37" s="23">
+        <v>60</v>
+      </c>
+      <c r="C37" s="23">
+        <v>180</v>
+      </c>
+      <c r="D37" s="32">
+        <v>1</v>
+      </c>
+      <c r="E37" s="32">
+        <v>0</v>
+      </c>
+      <c r="F37" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="G37" s="32"/>
+      <c r="H37" s="33"/>
+    </row>
+    <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="52">
+        <v>10</v>
+      </c>
+      <c r="B38" s="25">
+        <v>60</v>
+      </c>
+      <c r="C38" s="25">
+        <v>200</v>
+      </c>
+      <c r="D38" s="48">
+        <v>1</v>
+      </c>
+      <c r="E38" s="48">
+        <v>0</v>
+      </c>
+      <c r="F38" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="G38" s="48"/>
+      <c r="H38" s="49"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A21:H21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updating validation set results
</commit_message>
<xml_diff>
--- a/GHT/validation_set_results.xlsx
+++ b/GHT/validation_set_results.xlsx
@@ -4,21 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Interim Report" sheetId="1" r:id="rId1"/>
-    <sheet name="Power 4 Prior + Top 5 Avg" sheetId="4" r:id="rId2"/>
-    <sheet name="No Prior + Top 5 Avg" sheetId="5" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
+    <sheet name="No Prior + Top 5 Avg" sheetId="4" r:id="rId2"/>
+    <sheet name="Power 4 Prior + Top 5 Avg" sheetId="7" r:id="rId3"/>
+    <sheet name="Power 2 Prior + Top 5 Avg" sheetId="8" r:id="rId4"/>
+    <sheet name="No Prior + Top NMS Point" sheetId="5" r:id="rId5"/>
+    <sheet name="Power 4 Prior + Top NMS Point" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="17">
   <si>
     <t>Min Canny</t>
   </si>
@@ -63,6 +64,12 @@
   </si>
   <si>
     <t>Validation Set Result for C1 Spine Detection: No Prior + Top 5 Avg</t>
+  </si>
+  <si>
+    <t>The use of no prior caused a huge problem in 9136320</t>
+  </si>
+  <si>
+    <t>Validation Set Result for C1 Spine Detection: Power 4 Prior Prior + Top 5 Avg</t>
   </si>
 </sst>
 </file>
@@ -350,6 +357,15 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -368,15 +384,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -683,8 +690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G68" sqref="G68"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,16 +706,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="42"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="51"/>
     </row>
     <row r="2" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
@@ -1369,16 +1376,16 @@
     </row>
     <row r="29" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="30" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A30" s="43" t="s">
+      <c r="A30" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="44"/>
-      <c r="C30" s="44"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="45"/>
+      <c r="B30" s="53"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="53"/>
+      <c r="G30" s="53"/>
+      <c r="H30" s="54"/>
       <c r="J30" t="s">
         <v>11</v>
       </c>
@@ -1997,16 +2004,16 @@
     </row>
     <row r="58" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="40" t="s">
+      <c r="A59" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B59" s="41"/>
-      <c r="C59" s="41"/>
-      <c r="D59" s="41"/>
-      <c r="E59" s="41"/>
-      <c r="F59" s="41"/>
-      <c r="G59" s="41"/>
-      <c r="H59" s="42"/>
+      <c r="B59" s="50"/>
+      <c r="C59" s="50"/>
+      <c r="D59" s="50"/>
+      <c r="E59" s="50"/>
+      <c r="F59" s="50"/>
+      <c r="G59" s="50"/>
+      <c r="H59" s="51"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
@@ -2359,10 +2366,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2376,19 +2383,19 @@
     <col min="10" max="10" width="52.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A1" s="40" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="42"/>
-    </row>
-    <row r="2" spans="1:10" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="49" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="51"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
@@ -2416,8 +2423,14 @@
       <c r="J2" s="22" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L2" s="14">
+        <v>1071</v>
+      </c>
+      <c r="M2" s="47">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>5</v>
       </c>
@@ -2437,13 +2450,19 @@
         <v>0.5</v>
       </c>
       <c r="G3" s="14">
-        <v>1071</v>
-      </c>
-      <c r="H3" s="53">
+        <v>1078</v>
+      </c>
+      <c r="H3" s="47">
         <v>91</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L3" s="14">
+        <v>1327</v>
+      </c>
+      <c r="M3" s="47">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>5</v>
       </c>
@@ -2462,14 +2481,16 @@
       <c r="F4" s="13">
         <v>0.5</v>
       </c>
-      <c r="G4" s="14">
-        <v>1327</v>
-      </c>
-      <c r="H4" s="53">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G4" s="14"/>
+      <c r="H4" s="47"/>
+      <c r="L4" s="14">
+        <v>1198</v>
+      </c>
+      <c r="M4" s="47">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>5</v>
       </c>
@@ -2488,14 +2509,16 @@
       <c r="F5" s="13">
         <v>0.5</v>
       </c>
-      <c r="G5" s="14">
-        <v>1198</v>
-      </c>
-      <c r="H5" s="53">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G5" s="14"/>
+      <c r="H5" s="47"/>
+      <c r="L5" s="14">
+        <v>1369</v>
+      </c>
+      <c r="M5" s="47">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>5</v>
       </c>
@@ -2514,14 +2537,16 @@
       <c r="F6" s="13">
         <v>0.5</v>
       </c>
-      <c r="G6" s="14">
-        <v>1369</v>
-      </c>
-      <c r="H6" s="53">
+      <c r="G6" s="14"/>
+      <c r="H6" s="47"/>
+      <c r="L6" s="9">
+        <v>979</v>
+      </c>
+      <c r="M6" s="48">
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -2540,14 +2565,16 @@
       <c r="F7" s="8">
         <v>0.5</v>
       </c>
-      <c r="G7" s="9">
-        <v>979</v>
-      </c>
-      <c r="H7" s="54">
+      <c r="G7" s="9"/>
+      <c r="H7" s="48"/>
+      <c r="L7" s="9">
+        <v>1120</v>
+      </c>
+      <c r="M7" s="48">
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -2566,14 +2593,16 @@
       <c r="F8" s="8">
         <v>0.5</v>
       </c>
-      <c r="G8" s="9">
-        <v>1120</v>
-      </c>
-      <c r="H8" s="54">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G8" s="9"/>
+      <c r="H8" s="48"/>
+      <c r="L8" s="9">
+        <v>1049</v>
+      </c>
+      <c r="M8" s="48">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>5</v>
       </c>
@@ -2592,14 +2621,16 @@
       <c r="F9" s="8">
         <v>0.5</v>
       </c>
-      <c r="G9" s="9">
-        <v>1049</v>
-      </c>
-      <c r="H9" s="54">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G9" s="9"/>
+      <c r="H9" s="48"/>
+      <c r="L9" s="9">
+        <v>1265</v>
+      </c>
+      <c r="M9" s="48">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>5</v>
       </c>
@@ -2618,14 +2649,16 @@
       <c r="F10" s="8">
         <v>0.5</v>
       </c>
-      <c r="G10" s="9">
-        <v>1265</v>
-      </c>
-      <c r="H10" s="54">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G10" s="9"/>
+      <c r="H10" s="48"/>
+      <c r="L10" s="14">
+        <v>979</v>
+      </c>
+      <c r="M10" s="47">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>5</v>
       </c>
@@ -2645,9 +2678,15 @@
         <v>0.5</v>
       </c>
       <c r="G11" s="14"/>
-      <c r="H11" s="53"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H11" s="47"/>
+      <c r="L11" s="14">
+        <v>1043</v>
+      </c>
+      <c r="M11" s="47">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>5</v>
       </c>
@@ -2667,9 +2706,15 @@
         <v>0.5</v>
       </c>
       <c r="G12" s="14"/>
-      <c r="H12" s="53"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H12" s="47"/>
+      <c r="L12" s="14">
+        <v>1104</v>
+      </c>
+      <c r="M12" s="47">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>5</v>
       </c>
@@ -2689,9 +2734,15 @@
         <v>0.5</v>
       </c>
       <c r="G13" s="14"/>
-      <c r="H13" s="53"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H13" s="47"/>
+      <c r="L13" s="14">
+        <v>1184</v>
+      </c>
+      <c r="M13" s="47">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>5</v>
       </c>
@@ -2711,9 +2762,15 @@
         <v>0.5</v>
       </c>
       <c r="G14" s="14"/>
-      <c r="H14" s="53"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H14" s="47"/>
+      <c r="L14" s="9">
+        <v>1043</v>
+      </c>
+      <c r="M14" s="10">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>5</v>
       </c>
@@ -2734,8 +2791,14 @@
       </c>
       <c r="G15" s="9"/>
       <c r="H15" s="10"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L15" s="9">
+        <v>1292</v>
+      </c>
+      <c r="M15" s="10">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>5</v>
       </c>
@@ -2756,8 +2819,14 @@
       </c>
       <c r="G16" s="9"/>
       <c r="H16" s="10"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L16" s="9">
+        <v>1508</v>
+      </c>
+      <c r="M16" s="10">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <v>5</v>
       </c>
@@ -2778,8 +2847,14 @@
       </c>
       <c r="G17" s="9"/>
       <c r="H17" s="10"/>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L17" s="19">
+        <v>1823</v>
+      </c>
+      <c r="M17" s="20">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="17">
         <v>5</v>
       </c>
@@ -2801,20 +2876,20 @@
       <c r="G18" s="19"/>
       <c r="H18" s="20"/>
     </row>
-    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="40" t="s">
+    <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="41"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="41"/>
-      <c r="H21" s="42"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="50"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="50"/>
+      <c r="H21" s="51"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>8</v>
       </c>
@@ -2840,7 +2915,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>10</v>
       </c>
@@ -2860,9 +2935,9 @@
         <v>0.5</v>
       </c>
       <c r="G23" s="14"/>
-      <c r="H23" s="53"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H23" s="47"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>10</v>
       </c>
@@ -2882,9 +2957,9 @@
         <v>0.5</v>
       </c>
       <c r="G24" s="14"/>
-      <c r="H24" s="53"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H24" s="47"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>10</v>
       </c>
@@ -2904,9 +2979,9 @@
         <v>0.5</v>
       </c>
       <c r="G25" s="14"/>
-      <c r="H25" s="53"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H25" s="47"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>10</v>
       </c>
@@ -2926,9 +3001,9 @@
         <v>0.5</v>
       </c>
       <c r="G26" s="14"/>
-      <c r="H26" s="53"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H26" s="47"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>10</v>
       </c>
@@ -2948,9 +3023,9 @@
         <v>0.5</v>
       </c>
       <c r="G27" s="9"/>
-      <c r="H27" s="54"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H27" s="48"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <v>10</v>
       </c>
@@ -2970,9 +3045,9 @@
         <v>0.5</v>
       </c>
       <c r="G28" s="9"/>
-      <c r="H28" s="54"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H28" s="48"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>10</v>
       </c>
@@ -2992,9 +3067,9 @@
         <v>0.5</v>
       </c>
       <c r="G29" s="9"/>
-      <c r="H29" s="54"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H29" s="48"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <v>10</v>
       </c>
@@ -3014,9 +3089,9 @@
         <v>0.5</v>
       </c>
       <c r="G30" s="9"/>
-      <c r="H30" s="54"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H30" s="48"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <v>10</v>
       </c>
@@ -3036,9 +3111,9 @@
         <v>0.5</v>
       </c>
       <c r="G31" s="14"/>
-      <c r="H31" s="53"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H31" s="47"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>10</v>
       </c>
@@ -3058,7 +3133,7 @@
         <v>0.5</v>
       </c>
       <c r="G32" s="14"/>
-      <c r="H32" s="53"/>
+      <c r="H32" s="47"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
@@ -3080,7 +3155,7 @@
         <v>0.5</v>
       </c>
       <c r="G33" s="14"/>
-      <c r="H33" s="53"/>
+      <c r="H33" s="47"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
@@ -3102,7 +3177,7 @@
         <v>0.5</v>
       </c>
       <c r="G34" s="14"/>
-      <c r="H34" s="53"/>
+      <c r="H34" s="47"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
@@ -3180,7 +3255,7 @@
       <c r="C38" s="25">
         <v>200</v>
       </c>
-      <c r="D38" s="48">
+      <c r="D38" s="42">
         <v>1</v>
       </c>
       <c r="E38" s="19">
@@ -3206,8 +3281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3222,16 +3297,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="42"/>
+      <c r="A1" s="49" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="51"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -3282,9 +3357,9 @@
         <v>0.5</v>
       </c>
       <c r="G3" s="14">
-        <v>891</v>
-      </c>
-      <c r="H3" s="53">
+        <v>1077</v>
+      </c>
+      <c r="H3" s="47">
         <v>91</v>
       </c>
     </row>
@@ -3307,12 +3382,8 @@
       <c r="F4" s="13">
         <v>0.5</v>
       </c>
-      <c r="G4" s="14">
-        <v>1120</v>
-      </c>
-      <c r="H4" s="53">
-        <v>91</v>
-      </c>
+      <c r="G4" s="14"/>
+      <c r="H4" s="47"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
@@ -3334,7 +3405,7 @@
         <v>0.5</v>
       </c>
       <c r="G5" s="14"/>
-      <c r="H5" s="53"/>
+      <c r="H5" s="47"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
@@ -3356,7 +3427,7 @@
         <v>0.5</v>
       </c>
       <c r="G6" s="14"/>
-      <c r="H6" s="53"/>
+      <c r="H6" s="47"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
@@ -3378,7 +3449,7 @@
         <v>0.5</v>
       </c>
       <c r="G7" s="9"/>
-      <c r="H7" s="54"/>
+      <c r="H7" s="48"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
@@ -3400,7 +3471,7 @@
         <v>0.5</v>
       </c>
       <c r="G8" s="9"/>
-      <c r="H8" s="54"/>
+      <c r="H8" s="48"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
@@ -3422,7 +3493,7 @@
         <v>0.5</v>
       </c>
       <c r="G9" s="9"/>
-      <c r="H9" s="54"/>
+      <c r="H9" s="48"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
@@ -3444,7 +3515,7 @@
         <v>0.5</v>
       </c>
       <c r="G10" s="9"/>
-      <c r="H10" s="54"/>
+      <c r="H10" s="48"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
@@ -3466,7 +3537,7 @@
         <v>0.5</v>
       </c>
       <c r="G11" s="14"/>
-      <c r="H11" s="53"/>
+      <c r="H11" s="47"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
@@ -3488,7 +3559,7 @@
         <v>0.5</v>
       </c>
       <c r="G12" s="14"/>
-      <c r="H12" s="53"/>
+      <c r="H12" s="47"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
@@ -3510,7 +3581,7 @@
         <v>0.5</v>
       </c>
       <c r="G13" s="14"/>
-      <c r="H13" s="53"/>
+      <c r="H13" s="47"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
@@ -3532,7 +3603,7 @@
         <v>0.5</v>
       </c>
       <c r="G14" s="14"/>
-      <c r="H14" s="53"/>
+      <c r="H14" s="47"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
@@ -3624,16 +3695,16 @@
     </row>
     <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="40" t="s">
+      <c r="A21" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="41"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="41"/>
-      <c r="H21" s="42"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="50"/>
+      <c r="H21" s="51"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
@@ -3662,7 +3733,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="46">
+      <c r="A23" s="40">
         <v>10</v>
       </c>
       <c r="B23" s="24">
@@ -3680,11 +3751,15 @@
       <c r="F23" s="24">
         <v>0.5</v>
       </c>
-      <c r="G23" s="30"/>
-      <c r="H23" s="50"/>
+      <c r="G23" s="30">
+        <v>687</v>
+      </c>
+      <c r="H23" s="44">
+        <v>93</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="46">
+      <c r="A24" s="40">
         <v>10</v>
       </c>
       <c r="B24" s="24">
@@ -3702,11 +3777,15 @@
       <c r="F24" s="24">
         <v>0.5</v>
       </c>
-      <c r="G24" s="30"/>
-      <c r="H24" s="50"/>
+      <c r="G24" s="30">
+        <v>554</v>
+      </c>
+      <c r="H24" s="44">
+        <v>97</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="46">
+      <c r="A25" s="40">
         <v>10</v>
       </c>
       <c r="B25" s="24">
@@ -3724,11 +3803,15 @@
       <c r="F25" s="24">
         <v>0.5</v>
       </c>
-      <c r="G25" s="30"/>
-      <c r="H25" s="50"/>
+      <c r="G25" s="30">
+        <v>564</v>
+      </c>
+      <c r="H25" s="44">
+        <v>97</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="46">
+      <c r="A26" s="40">
         <v>10</v>
       </c>
       <c r="B26" s="24">
@@ -3746,11 +3829,15 @@
       <c r="F26" s="24">
         <v>0.5</v>
       </c>
-      <c r="G26" s="30"/>
-      <c r="H26" s="50"/>
+      <c r="G26" s="30">
+        <v>660</v>
+      </c>
+      <c r="H26" s="44">
+        <v>95</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="47">
+      <c r="A27" s="41">
         <v>10</v>
       </c>
       <c r="B27" s="23">
@@ -3768,11 +3855,15 @@
       <c r="F27" s="23">
         <v>0.5</v>
       </c>
-      <c r="G27" s="32"/>
-      <c r="H27" s="51"/>
+      <c r="G27" s="32">
+        <v>707</v>
+      </c>
+      <c r="H27" s="45">
+        <v>95</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="47">
+      <c r="A28" s="41">
         <v>10</v>
       </c>
       <c r="B28" s="23">
@@ -3790,11 +3881,15 @@
       <c r="F28" s="23">
         <v>0.5</v>
       </c>
-      <c r="G28" s="32"/>
-      <c r="H28" s="51"/>
+      <c r="G28" s="32">
+        <v>565</v>
+      </c>
+      <c r="H28" s="45">
+        <v>97</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="47">
+      <c r="A29" s="41">
         <v>10</v>
       </c>
       <c r="B29" s="23">
@@ -3812,11 +3907,15 @@
       <c r="F29" s="23">
         <v>0.5</v>
       </c>
-      <c r="G29" s="32"/>
-      <c r="H29" s="51"/>
+      <c r="G29" s="32">
+        <v>537</v>
+      </c>
+      <c r="H29" s="45">
+        <v>97</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="47">
+      <c r="A30" s="41">
         <v>10</v>
       </c>
       <c r="B30" s="23">
@@ -3834,11 +3933,15 @@
       <c r="F30" s="23">
         <v>0.5</v>
       </c>
-      <c r="G30" s="32"/>
-      <c r="H30" s="51"/>
+      <c r="G30" s="32">
+        <v>627</v>
+      </c>
+      <c r="H30" s="45">
+        <v>96</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="46">
+      <c r="A31" s="40">
         <v>10</v>
       </c>
       <c r="B31" s="24">
@@ -3857,10 +3960,10 @@
         <v>0.5</v>
       </c>
       <c r="G31" s="30"/>
-      <c r="H31" s="50"/>
+      <c r="H31" s="44"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="46">
+      <c r="A32" s="40">
         <v>10</v>
       </c>
       <c r="B32" s="24">
@@ -3879,10 +3982,10 @@
         <v>0.5</v>
       </c>
       <c r="G32" s="30"/>
-      <c r="H32" s="50"/>
+      <c r="H32" s="44"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="46">
+      <c r="A33" s="40">
         <v>10</v>
       </c>
       <c r="B33" s="24">
@@ -3901,10 +4004,10 @@
         <v>0.5</v>
       </c>
       <c r="G33" s="30"/>
-      <c r="H33" s="50"/>
+      <c r="H33" s="44"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="46">
+      <c r="A34" s="40">
         <v>10</v>
       </c>
       <c r="B34" s="24">
@@ -3923,10 +4026,10 @@
         <v>0.5</v>
       </c>
       <c r="G34" s="30"/>
-      <c r="H34" s="50"/>
+      <c r="H34" s="44"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="47">
+      <c r="A35" s="41">
         <v>10</v>
       </c>
       <c r="B35" s="23">
@@ -3948,7 +4051,7 @@
       <c r="H35" s="33"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="47">
+      <c r="A36" s="41">
         <v>10</v>
       </c>
       <c r="B36" s="23">
@@ -3970,7 +4073,7 @@
       <c r="H36" s="33"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="47">
+      <c r="A37" s="41">
         <v>10</v>
       </c>
       <c r="B37" s="23">
@@ -3992,7 +4095,7 @@
       <c r="H37" s="33"/>
     </row>
     <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="52">
+      <c r="A38" s="46">
         <v>10</v>
       </c>
       <c r="B38" s="25">
@@ -4001,17 +4104,17 @@
       <c r="C38" s="25">
         <v>200</v>
       </c>
-      <c r="D38" s="48">
-        <v>1</v>
-      </c>
-      <c r="E38" s="48">
+      <c r="D38" s="42">
+        <v>1</v>
+      </c>
+      <c r="E38" s="42">
         <v>0</v>
       </c>
       <c r="F38" s="25">
         <v>0.5</v>
       </c>
-      <c r="G38" s="48"/>
-      <c r="H38" s="49"/>
+      <c r="G38" s="42"/>
+      <c r="H38" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4025,24 +4128,2542 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="1" customWidth="1"/>
+    <col min="5" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="52.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="49" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="51"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
+        <v>5</v>
+      </c>
+      <c r="B3" s="13">
+        <v>30</v>
+      </c>
+      <c r="C3" s="24">
+        <v>140</v>
+      </c>
+      <c r="D3" s="14">
+        <v>1</v>
+      </c>
+      <c r="E3" s="14">
+        <v>0</v>
+      </c>
+      <c r="F3" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G3" s="14">
+        <v>1082</v>
+      </c>
+      <c r="H3" s="47">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>5</v>
+      </c>
+      <c r="B4" s="13">
+        <v>30</v>
+      </c>
+      <c r="C4" s="24">
+        <v>160</v>
+      </c>
+      <c r="D4" s="14">
+        <v>1</v>
+      </c>
+      <c r="E4" s="14">
+        <v>0</v>
+      </c>
+      <c r="F4" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="14"/>
+      <c r="H4" s="47"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>5</v>
+      </c>
+      <c r="B5" s="13">
+        <v>30</v>
+      </c>
+      <c r="C5" s="24">
+        <v>180</v>
+      </c>
+      <c r="D5" s="14">
+        <v>1</v>
+      </c>
+      <c r="E5" s="14">
+        <v>0</v>
+      </c>
+      <c r="F5" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G5" s="14"/>
+      <c r="H5" s="47"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" s="13">
+        <v>30</v>
+      </c>
+      <c r="C6" s="24">
+        <v>200</v>
+      </c>
+      <c r="D6" s="14">
+        <v>1</v>
+      </c>
+      <c r="E6" s="14">
+        <v>0</v>
+      </c>
+      <c r="F6" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G6" s="14"/>
+      <c r="H6" s="47"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="8">
+        <v>40</v>
+      </c>
+      <c r="C7" s="23">
+        <v>140</v>
+      </c>
+      <c r="D7" s="9">
+        <v>1</v>
+      </c>
+      <c r="E7" s="9">
+        <v>0</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G7" s="9"/>
+      <c r="H7" s="48"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>5</v>
+      </c>
+      <c r="B8" s="8">
+        <v>40</v>
+      </c>
+      <c r="C8" s="23">
+        <v>160</v>
+      </c>
+      <c r="D8" s="9">
+        <v>1</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G8" s="9"/>
+      <c r="H8" s="48"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>5</v>
+      </c>
+      <c r="B9" s="8">
+        <v>40</v>
+      </c>
+      <c r="C9" s="23">
+        <v>180</v>
+      </c>
+      <c r="D9" s="9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="9">
+        <v>0</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G9" s="9"/>
+      <c r="H9" s="48"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>5</v>
+      </c>
+      <c r="B10" s="8">
+        <v>40</v>
+      </c>
+      <c r="C10" s="23">
+        <v>200</v>
+      </c>
+      <c r="D10" s="9">
+        <v>1</v>
+      </c>
+      <c r="E10" s="9">
+        <v>0</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="9"/>
+      <c r="H10" s="48"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>5</v>
+      </c>
+      <c r="B11" s="13">
+        <v>50</v>
+      </c>
+      <c r="C11" s="24">
+        <v>140</v>
+      </c>
+      <c r="D11" s="14">
+        <v>1</v>
+      </c>
+      <c r="E11" s="14">
+        <v>0</v>
+      </c>
+      <c r="F11" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G11" s="14"/>
+      <c r="H11" s="47"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>5</v>
+      </c>
+      <c r="B12" s="13">
+        <v>50</v>
+      </c>
+      <c r="C12" s="24">
+        <v>160</v>
+      </c>
+      <c r="D12" s="14">
+        <v>1</v>
+      </c>
+      <c r="E12" s="14">
+        <v>0</v>
+      </c>
+      <c r="F12" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G12" s="14"/>
+      <c r="H12" s="47"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>5</v>
+      </c>
+      <c r="B13" s="13">
+        <v>50</v>
+      </c>
+      <c r="C13" s="24">
+        <v>180</v>
+      </c>
+      <c r="D13" s="14">
+        <v>1</v>
+      </c>
+      <c r="E13" s="14">
+        <v>0</v>
+      </c>
+      <c r="F13" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G13" s="14"/>
+      <c r="H13" s="47"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>5</v>
+      </c>
+      <c r="B14" s="13">
+        <v>50</v>
+      </c>
+      <c r="C14" s="24">
+        <v>200</v>
+      </c>
+      <c r="D14" s="14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="14">
+        <v>0</v>
+      </c>
+      <c r="F14" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G14" s="14"/>
+      <c r="H14" s="47"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>5</v>
+      </c>
+      <c r="B15" s="8">
+        <v>60</v>
+      </c>
+      <c r="C15" s="23">
+        <v>140</v>
+      </c>
+      <c r="D15" s="9">
+        <v>1</v>
+      </c>
+      <c r="E15" s="9">
+        <v>0</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G15" s="9"/>
+      <c r="H15" s="10"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>5</v>
+      </c>
+      <c r="B16" s="8">
+        <v>60</v>
+      </c>
+      <c r="C16" s="23">
+        <v>160</v>
+      </c>
+      <c r="D16" s="9">
+        <v>1</v>
+      </c>
+      <c r="E16" s="9">
+        <v>0</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G16" s="9"/>
+      <c r="H16" s="10"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>5</v>
+      </c>
+      <c r="B17" s="8">
+        <v>60</v>
+      </c>
+      <c r="C17" s="23">
+        <v>180</v>
+      </c>
+      <c r="D17" s="9">
+        <v>1</v>
+      </c>
+      <c r="E17" s="9">
+        <v>0</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G17" s="9"/>
+      <c r="H17" s="10"/>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="17">
+        <v>5</v>
+      </c>
+      <c r="B18" s="18">
+        <v>60</v>
+      </c>
+      <c r="C18" s="25">
+        <v>200</v>
+      </c>
+      <c r="D18" s="19">
+        <v>1</v>
+      </c>
+      <c r="E18" s="19">
+        <v>0</v>
+      </c>
+      <c r="F18" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="G18" s="19"/>
+      <c r="H18" s="20"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="50"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="50"/>
+      <c r="H21" s="51"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="40">
+        <v>10</v>
+      </c>
+      <c r="B23" s="24">
+        <v>30</v>
+      </c>
+      <c r="C23" s="24">
+        <v>140</v>
+      </c>
+      <c r="D23" s="30">
+        <v>1</v>
+      </c>
+      <c r="E23" s="30">
+        <v>0</v>
+      </c>
+      <c r="F23" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G23" s="30"/>
+      <c r="H23" s="44"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="40">
+        <v>10</v>
+      </c>
+      <c r="B24" s="24">
+        <v>30</v>
+      </c>
+      <c r="C24" s="24">
+        <v>160</v>
+      </c>
+      <c r="D24" s="30">
+        <v>1</v>
+      </c>
+      <c r="E24" s="30">
+        <v>0</v>
+      </c>
+      <c r="F24" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G24" s="30"/>
+      <c r="H24" s="44"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="40">
+        <v>10</v>
+      </c>
+      <c r="B25" s="24">
+        <v>30</v>
+      </c>
+      <c r="C25" s="24">
+        <v>180</v>
+      </c>
+      <c r="D25" s="30">
+        <v>1</v>
+      </c>
+      <c r="E25" s="30">
+        <v>0</v>
+      </c>
+      <c r="F25" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G25" s="30"/>
+      <c r="H25" s="44"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="40">
+        <v>10</v>
+      </c>
+      <c r="B26" s="24">
+        <v>30</v>
+      </c>
+      <c r="C26" s="24">
+        <v>200</v>
+      </c>
+      <c r="D26" s="30">
+        <v>1</v>
+      </c>
+      <c r="E26" s="30">
+        <v>0</v>
+      </c>
+      <c r="F26" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G26" s="30"/>
+      <c r="H26" s="44"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="41">
+        <v>10</v>
+      </c>
+      <c r="B27" s="23">
+        <v>40</v>
+      </c>
+      <c r="C27" s="23">
+        <v>140</v>
+      </c>
+      <c r="D27" s="32">
+        <v>1</v>
+      </c>
+      <c r="E27" s="32">
+        <v>0</v>
+      </c>
+      <c r="F27" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="G27" s="32"/>
+      <c r="H27" s="45"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="41">
+        <v>10</v>
+      </c>
+      <c r="B28" s="23">
+        <v>40</v>
+      </c>
+      <c r="C28" s="23">
+        <v>160</v>
+      </c>
+      <c r="D28" s="32">
+        <v>1</v>
+      </c>
+      <c r="E28" s="32">
+        <v>0</v>
+      </c>
+      <c r="F28" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="G28" s="32"/>
+      <c r="H28" s="45"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="41">
+        <v>10</v>
+      </c>
+      <c r="B29" s="23">
+        <v>40</v>
+      </c>
+      <c r="C29" s="23">
+        <v>180</v>
+      </c>
+      <c r="D29" s="32">
+        <v>1</v>
+      </c>
+      <c r="E29" s="32">
+        <v>0</v>
+      </c>
+      <c r="F29" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="G29" s="32"/>
+      <c r="H29" s="45"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="41">
+        <v>10</v>
+      </c>
+      <c r="B30" s="23">
+        <v>40</v>
+      </c>
+      <c r="C30" s="23">
+        <v>200</v>
+      </c>
+      <c r="D30" s="32">
+        <v>1</v>
+      </c>
+      <c r="E30" s="32">
+        <v>0</v>
+      </c>
+      <c r="F30" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="G30" s="32"/>
+      <c r="H30" s="45"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="40">
+        <v>10</v>
+      </c>
+      <c r="B31" s="24">
+        <v>50</v>
+      </c>
+      <c r="C31" s="24">
+        <v>140</v>
+      </c>
+      <c r="D31" s="30">
+        <v>1</v>
+      </c>
+      <c r="E31" s="30">
+        <v>0</v>
+      </c>
+      <c r="F31" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G31" s="30"/>
+      <c r="H31" s="44"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="40">
+        <v>10</v>
+      </c>
+      <c r="B32" s="24">
+        <v>50</v>
+      </c>
+      <c r="C32" s="24">
+        <v>160</v>
+      </c>
+      <c r="D32" s="30">
+        <v>1</v>
+      </c>
+      <c r="E32" s="30">
+        <v>0</v>
+      </c>
+      <c r="F32" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G32" s="30"/>
+      <c r="H32" s="44"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="40">
+        <v>10</v>
+      </c>
+      <c r="B33" s="24">
+        <v>50</v>
+      </c>
+      <c r="C33" s="24">
+        <v>180</v>
+      </c>
+      <c r="D33" s="30">
+        <v>1</v>
+      </c>
+      <c r="E33" s="30">
+        <v>0</v>
+      </c>
+      <c r="F33" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G33" s="30"/>
+      <c r="H33" s="44"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="40">
+        <v>10</v>
+      </c>
+      <c r="B34" s="24">
+        <v>50</v>
+      </c>
+      <c r="C34" s="24">
+        <v>200</v>
+      </c>
+      <c r="D34" s="30">
+        <v>1</v>
+      </c>
+      <c r="E34" s="30">
+        <v>0</v>
+      </c>
+      <c r="F34" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G34" s="30"/>
+      <c r="H34" s="44"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="41">
+        <v>10</v>
+      </c>
+      <c r="B35" s="23">
+        <v>60</v>
+      </c>
+      <c r="C35" s="23">
+        <v>140</v>
+      </c>
+      <c r="D35" s="32">
+        <v>1</v>
+      </c>
+      <c r="E35" s="32">
+        <v>0</v>
+      </c>
+      <c r="F35" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="G35" s="32"/>
+      <c r="H35" s="33"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="41">
+        <v>10</v>
+      </c>
+      <c r="B36" s="23">
+        <v>60</v>
+      </c>
+      <c r="C36" s="23">
+        <v>160</v>
+      </c>
+      <c r="D36" s="32">
+        <v>1</v>
+      </c>
+      <c r="E36" s="32">
+        <v>0</v>
+      </c>
+      <c r="F36" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="G36" s="32"/>
+      <c r="H36" s="33"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="41">
+        <v>10</v>
+      </c>
+      <c r="B37" s="23">
+        <v>60</v>
+      </c>
+      <c r="C37" s="23">
+        <v>180</v>
+      </c>
+      <c r="D37" s="32">
+        <v>1</v>
+      </c>
+      <c r="E37" s="32">
+        <v>0</v>
+      </c>
+      <c r="F37" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="G37" s="32"/>
+      <c r="H37" s="33"/>
+    </row>
+    <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="46">
+        <v>10</v>
+      </c>
+      <c r="B38" s="25">
+        <v>60</v>
+      </c>
+      <c r="C38" s="25">
+        <v>200</v>
+      </c>
+      <c r="D38" s="42">
+        <v>1</v>
+      </c>
+      <c r="E38" s="42">
+        <v>0</v>
+      </c>
+      <c r="F38" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="G38" s="42"/>
+      <c r="H38" s="43"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A21:H21"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3:H10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="1" customWidth="1"/>
+    <col min="5" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="52.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="49" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="51"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
+        <v>5</v>
+      </c>
+      <c r="B3" s="13">
+        <v>30</v>
+      </c>
+      <c r="C3" s="24">
+        <v>140</v>
+      </c>
+      <c r="D3" s="14">
+        <v>1</v>
+      </c>
+      <c r="E3" s="14">
+        <v>0</v>
+      </c>
+      <c r="F3" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G3" s="14">
+        <v>891</v>
+      </c>
+      <c r="H3" s="47">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>5</v>
+      </c>
+      <c r="B4" s="13">
+        <v>30</v>
+      </c>
+      <c r="C4" s="24">
+        <v>160</v>
+      </c>
+      <c r="D4" s="14">
+        <v>1</v>
+      </c>
+      <c r="E4" s="14">
+        <v>0</v>
+      </c>
+      <c r="F4" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="14">
+        <v>1120</v>
+      </c>
+      <c r="H4" s="47">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>5</v>
+      </c>
+      <c r="B5" s="13">
+        <v>30</v>
+      </c>
+      <c r="C5" s="24">
+        <v>180</v>
+      </c>
+      <c r="D5" s="14">
+        <v>1</v>
+      </c>
+      <c r="E5" s="14">
+        <v>0</v>
+      </c>
+      <c r="F5" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G5" s="14">
+        <v>1143</v>
+      </c>
+      <c r="H5" s="47">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" s="13">
+        <v>30</v>
+      </c>
+      <c r="C6" s="24">
+        <v>200</v>
+      </c>
+      <c r="D6" s="14">
+        <v>1</v>
+      </c>
+      <c r="E6" s="14">
+        <v>0</v>
+      </c>
+      <c r="F6" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G6" s="14">
+        <v>1368</v>
+      </c>
+      <c r="H6" s="47">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="8">
+        <v>40</v>
+      </c>
+      <c r="C7" s="23">
+        <v>140</v>
+      </c>
+      <c r="D7" s="9">
+        <v>1</v>
+      </c>
+      <c r="E7" s="9">
+        <v>0</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G7" s="9">
+        <v>850</v>
+      </c>
+      <c r="H7" s="48">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>5</v>
+      </c>
+      <c r="B8" s="8">
+        <v>40</v>
+      </c>
+      <c r="C8" s="23">
+        <v>160</v>
+      </c>
+      <c r="D8" s="9">
+        <v>1</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G8" s="9">
+        <v>700</v>
+      </c>
+      <c r="H8" s="48">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>5</v>
+      </c>
+      <c r="B9" s="8">
+        <v>40</v>
+      </c>
+      <c r="C9" s="23">
+        <v>180</v>
+      </c>
+      <c r="D9" s="9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="9">
+        <v>0</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G9" s="9">
+        <v>1035</v>
+      </c>
+      <c r="H9" s="48">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>5</v>
+      </c>
+      <c r="B10" s="8">
+        <v>40</v>
+      </c>
+      <c r="C10" s="23">
+        <v>200</v>
+      </c>
+      <c r="D10" s="9">
+        <v>1</v>
+      </c>
+      <c r="E10" s="9">
+        <v>0</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="9">
+        <v>825</v>
+      </c>
+      <c r="H10" s="48">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>5</v>
+      </c>
+      <c r="B11" s="13">
+        <v>50</v>
+      </c>
+      <c r="C11" s="24">
+        <v>140</v>
+      </c>
+      <c r="D11" s="14">
+        <v>1</v>
+      </c>
+      <c r="E11" s="14">
+        <v>0</v>
+      </c>
+      <c r="F11" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G11" s="14">
+        <v>787</v>
+      </c>
+      <c r="H11" s="47">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>5</v>
+      </c>
+      <c r="B12" s="13">
+        <v>50</v>
+      </c>
+      <c r="C12" s="24">
+        <v>160</v>
+      </c>
+      <c r="D12" s="14">
+        <v>1</v>
+      </c>
+      <c r="E12" s="14">
+        <v>0</v>
+      </c>
+      <c r="F12" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G12" s="14">
+        <v>1950</v>
+      </c>
+      <c r="H12" s="47">
+        <v>94</v>
+      </c>
+      <c r="J12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>5</v>
+      </c>
+      <c r="B13" s="13">
+        <v>50</v>
+      </c>
+      <c r="C13" s="24">
+        <v>180</v>
+      </c>
+      <c r="D13" s="14">
+        <v>1</v>
+      </c>
+      <c r="E13" s="14">
+        <v>0</v>
+      </c>
+      <c r="F13" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G13" s="14">
+        <v>905</v>
+      </c>
+      <c r="H13" s="47">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>5</v>
+      </c>
+      <c r="B14" s="13">
+        <v>50</v>
+      </c>
+      <c r="C14" s="24">
+        <v>200</v>
+      </c>
+      <c r="D14" s="14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="14">
+        <v>0</v>
+      </c>
+      <c r="F14" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G14" s="14">
+        <v>3469</v>
+      </c>
+      <c r="H14" s="47">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>5</v>
+      </c>
+      <c r="B15" s="8">
+        <v>60</v>
+      </c>
+      <c r="C15" s="23">
+        <v>140</v>
+      </c>
+      <c r="D15" s="9">
+        <v>1</v>
+      </c>
+      <c r="E15" s="9">
+        <v>0</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G15" s="9">
+        <v>2937</v>
+      </c>
+      <c r="H15" s="10">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>5</v>
+      </c>
+      <c r="B16" s="8">
+        <v>60</v>
+      </c>
+      <c r="C16" s="23">
+        <v>160</v>
+      </c>
+      <c r="D16" s="9">
+        <v>1</v>
+      </c>
+      <c r="E16" s="9">
+        <v>0</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G16" s="9">
+        <v>4411</v>
+      </c>
+      <c r="H16" s="10">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>5</v>
+      </c>
+      <c r="B17" s="8">
+        <v>60</v>
+      </c>
+      <c r="C17" s="23">
+        <v>180</v>
+      </c>
+      <c r="D17" s="9">
+        <v>1</v>
+      </c>
+      <c r="E17" s="9">
+        <v>0</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G17" s="9">
+        <v>3436</v>
+      </c>
+      <c r="H17" s="10">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="17">
+        <v>5</v>
+      </c>
+      <c r="B18" s="18">
+        <v>60</v>
+      </c>
+      <c r="C18" s="25">
+        <v>200</v>
+      </c>
+      <c r="D18" s="19">
+        <v>1</v>
+      </c>
+      <c r="E18" s="19">
+        <v>0</v>
+      </c>
+      <c r="F18" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="G18" s="19">
+        <v>3529</v>
+      </c>
+      <c r="H18" s="20">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="50"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="50"/>
+      <c r="H21" s="51"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="40">
+        <v>10</v>
+      </c>
+      <c r="B23" s="24">
+        <v>30</v>
+      </c>
+      <c r="C23" s="24">
+        <v>140</v>
+      </c>
+      <c r="D23" s="30">
+        <v>1</v>
+      </c>
+      <c r="E23" s="30">
+        <v>0</v>
+      </c>
+      <c r="F23" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G23" s="30"/>
+      <c r="H23" s="44"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="40">
+        <v>10</v>
+      </c>
+      <c r="B24" s="24">
+        <v>30</v>
+      </c>
+      <c r="C24" s="24">
+        <v>160</v>
+      </c>
+      <c r="D24" s="30">
+        <v>1</v>
+      </c>
+      <c r="E24" s="30">
+        <v>0</v>
+      </c>
+      <c r="F24" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G24" s="30"/>
+      <c r="H24" s="44"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="40">
+        <v>10</v>
+      </c>
+      <c r="B25" s="24">
+        <v>30</v>
+      </c>
+      <c r="C25" s="24">
+        <v>180</v>
+      </c>
+      <c r="D25" s="30">
+        <v>1</v>
+      </c>
+      <c r="E25" s="30">
+        <v>0</v>
+      </c>
+      <c r="F25" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G25" s="30"/>
+      <c r="H25" s="44"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="40">
+        <v>10</v>
+      </c>
+      <c r="B26" s="24">
+        <v>30</v>
+      </c>
+      <c r="C26" s="24">
+        <v>200</v>
+      </c>
+      <c r="D26" s="30">
+        <v>1</v>
+      </c>
+      <c r="E26" s="30">
+        <v>0</v>
+      </c>
+      <c r="F26" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G26" s="30"/>
+      <c r="H26" s="44"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="41">
+        <v>10</v>
+      </c>
+      <c r="B27" s="23">
+        <v>40</v>
+      </c>
+      <c r="C27" s="23">
+        <v>140</v>
+      </c>
+      <c r="D27" s="32">
+        <v>1</v>
+      </c>
+      <c r="E27" s="32">
+        <v>0</v>
+      </c>
+      <c r="F27" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="G27" s="32"/>
+      <c r="H27" s="45"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="41">
+        <v>10</v>
+      </c>
+      <c r="B28" s="23">
+        <v>40</v>
+      </c>
+      <c r="C28" s="23">
+        <v>160</v>
+      </c>
+      <c r="D28" s="32">
+        <v>1</v>
+      </c>
+      <c r="E28" s="32">
+        <v>0</v>
+      </c>
+      <c r="F28" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="G28" s="32"/>
+      <c r="H28" s="45"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="41">
+        <v>10</v>
+      </c>
+      <c r="B29" s="23">
+        <v>40</v>
+      </c>
+      <c r="C29" s="23">
+        <v>180</v>
+      </c>
+      <c r="D29" s="32">
+        <v>1</v>
+      </c>
+      <c r="E29" s="32">
+        <v>0</v>
+      </c>
+      <c r="F29" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="G29" s="32"/>
+      <c r="H29" s="45"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="41">
+        <v>10</v>
+      </c>
+      <c r="B30" s="23">
+        <v>40</v>
+      </c>
+      <c r="C30" s="23">
+        <v>200</v>
+      </c>
+      <c r="D30" s="32">
+        <v>1</v>
+      </c>
+      <c r="E30" s="32">
+        <v>0</v>
+      </c>
+      <c r="F30" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="G30" s="32"/>
+      <c r="H30" s="45"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="40">
+        <v>10</v>
+      </c>
+      <c r="B31" s="24">
+        <v>50</v>
+      </c>
+      <c r="C31" s="24">
+        <v>140</v>
+      </c>
+      <c r="D31" s="30">
+        <v>1</v>
+      </c>
+      <c r="E31" s="30">
+        <v>0</v>
+      </c>
+      <c r="F31" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G31" s="30"/>
+      <c r="H31" s="44"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="40">
+        <v>10</v>
+      </c>
+      <c r="B32" s="24">
+        <v>50</v>
+      </c>
+      <c r="C32" s="24">
+        <v>160</v>
+      </c>
+      <c r="D32" s="30">
+        <v>1</v>
+      </c>
+      <c r="E32" s="30">
+        <v>0</v>
+      </c>
+      <c r="F32" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G32" s="30"/>
+      <c r="H32" s="44"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="40">
+        <v>10</v>
+      </c>
+      <c r="B33" s="24">
+        <v>50</v>
+      </c>
+      <c r="C33" s="24">
+        <v>180</v>
+      </c>
+      <c r="D33" s="30">
+        <v>1</v>
+      </c>
+      <c r="E33" s="30">
+        <v>0</v>
+      </c>
+      <c r="F33" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G33" s="30"/>
+      <c r="H33" s="44"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="40">
+        <v>10</v>
+      </c>
+      <c r="B34" s="24">
+        <v>50</v>
+      </c>
+      <c r="C34" s="24">
+        <v>200</v>
+      </c>
+      <c r="D34" s="30">
+        <v>1</v>
+      </c>
+      <c r="E34" s="30">
+        <v>0</v>
+      </c>
+      <c r="F34" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G34" s="30"/>
+      <c r="H34" s="44"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="41">
+        <v>10</v>
+      </c>
+      <c r="B35" s="23">
+        <v>60</v>
+      </c>
+      <c r="C35" s="23">
+        <v>140</v>
+      </c>
+      <c r="D35" s="32">
+        <v>1</v>
+      </c>
+      <c r="E35" s="32">
+        <v>0</v>
+      </c>
+      <c r="F35" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="G35" s="32"/>
+      <c r="H35" s="33"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="41">
+        <v>10</v>
+      </c>
+      <c r="B36" s="23">
+        <v>60</v>
+      </c>
+      <c r="C36" s="23">
+        <v>160</v>
+      </c>
+      <c r="D36" s="32">
+        <v>1</v>
+      </c>
+      <c r="E36" s="32">
+        <v>0</v>
+      </c>
+      <c r="F36" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="G36" s="32"/>
+      <c r="H36" s="33"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="41">
+        <v>10</v>
+      </c>
+      <c r="B37" s="23">
+        <v>60</v>
+      </c>
+      <c r="C37" s="23">
+        <v>180</v>
+      </c>
+      <c r="D37" s="32">
+        <v>1</v>
+      </c>
+      <c r="E37" s="32">
+        <v>0</v>
+      </c>
+      <c r="F37" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="G37" s="32"/>
+      <c r="H37" s="33"/>
+    </row>
+    <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="46">
+        <v>10</v>
+      </c>
+      <c r="B38" s="25">
+        <v>60</v>
+      </c>
+      <c r="C38" s="25">
+        <v>200</v>
+      </c>
+      <c r="D38" s="42">
+        <v>1</v>
+      </c>
+      <c r="E38" s="42">
+        <v>0</v>
+      </c>
+      <c r="F38" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="G38" s="42"/>
+      <c r="H38" s="43"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A21:H21"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="1" customWidth="1"/>
+    <col min="5" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="52.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="51"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
+        <v>5</v>
+      </c>
+      <c r="B3" s="13">
+        <v>30</v>
+      </c>
+      <c r="C3" s="24">
+        <v>140</v>
+      </c>
+      <c r="D3" s="14">
+        <v>1</v>
+      </c>
+      <c r="E3" s="14">
+        <v>0</v>
+      </c>
+      <c r="F3" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G3" s="14">
+        <v>891</v>
+      </c>
+      <c r="H3" s="47">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>5</v>
+      </c>
+      <c r="B4" s="13">
+        <v>30</v>
+      </c>
+      <c r="C4" s="24">
+        <v>160</v>
+      </c>
+      <c r="D4" s="14">
+        <v>1</v>
+      </c>
+      <c r="E4" s="14">
+        <v>0</v>
+      </c>
+      <c r="F4" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="14">
+        <v>1120</v>
+      </c>
+      <c r="H4" s="47">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>5</v>
+      </c>
+      <c r="B5" s="13">
+        <v>30</v>
+      </c>
+      <c r="C5" s="24">
+        <v>180</v>
+      </c>
+      <c r="D5" s="14">
+        <v>1</v>
+      </c>
+      <c r="E5" s="14">
+        <v>0</v>
+      </c>
+      <c r="F5" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G5" s="14">
+        <v>1143</v>
+      </c>
+      <c r="H5" s="47">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" s="13">
+        <v>30</v>
+      </c>
+      <c r="C6" s="24">
+        <v>200</v>
+      </c>
+      <c r="D6" s="14">
+        <v>1</v>
+      </c>
+      <c r="E6" s="14">
+        <v>0</v>
+      </c>
+      <c r="F6" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G6" s="14">
+        <v>1368</v>
+      </c>
+      <c r="H6" s="47">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="8">
+        <v>40</v>
+      </c>
+      <c r="C7" s="23">
+        <v>140</v>
+      </c>
+      <c r="D7" s="9">
+        <v>1</v>
+      </c>
+      <c r="E7" s="9">
+        <v>0</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G7" s="9">
+        <v>850</v>
+      </c>
+      <c r="H7" s="48">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>5</v>
+      </c>
+      <c r="B8" s="8">
+        <v>40</v>
+      </c>
+      <c r="C8" s="23">
+        <v>160</v>
+      </c>
+      <c r="D8" s="9">
+        <v>1</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G8" s="9">
+        <v>700</v>
+      </c>
+      <c r="H8" s="48">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>5</v>
+      </c>
+      <c r="B9" s="8">
+        <v>40</v>
+      </c>
+      <c r="C9" s="23">
+        <v>180</v>
+      </c>
+      <c r="D9" s="9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="9">
+        <v>0</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G9" s="9">
+        <v>1035</v>
+      </c>
+      <c r="H9" s="48">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>5</v>
+      </c>
+      <c r="B10" s="8">
+        <v>40</v>
+      </c>
+      <c r="C10" s="23">
+        <v>200</v>
+      </c>
+      <c r="D10" s="9">
+        <v>1</v>
+      </c>
+      <c r="E10" s="9">
+        <v>0</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="9">
+        <v>825</v>
+      </c>
+      <c r="H10" s="48">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>5</v>
+      </c>
+      <c r="B11" s="13">
+        <v>50</v>
+      </c>
+      <c r="C11" s="24">
+        <v>140</v>
+      </c>
+      <c r="D11" s="14">
+        <v>1</v>
+      </c>
+      <c r="E11" s="14">
+        <v>0</v>
+      </c>
+      <c r="F11" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G11" s="14"/>
+      <c r="H11" s="47"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>5</v>
+      </c>
+      <c r="B12" s="13">
+        <v>50</v>
+      </c>
+      <c r="C12" s="24">
+        <v>160</v>
+      </c>
+      <c r="D12" s="14">
+        <v>1</v>
+      </c>
+      <c r="E12" s="14">
+        <v>0</v>
+      </c>
+      <c r="F12" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G12" s="14"/>
+      <c r="H12" s="47"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>5</v>
+      </c>
+      <c r="B13" s="13">
+        <v>50</v>
+      </c>
+      <c r="C13" s="24">
+        <v>180</v>
+      </c>
+      <c r="D13" s="14">
+        <v>1</v>
+      </c>
+      <c r="E13" s="14">
+        <v>0</v>
+      </c>
+      <c r="F13" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G13" s="14"/>
+      <c r="H13" s="47"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>5</v>
+      </c>
+      <c r="B14" s="13">
+        <v>50</v>
+      </c>
+      <c r="C14" s="24">
+        <v>200</v>
+      </c>
+      <c r="D14" s="14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="14">
+        <v>0</v>
+      </c>
+      <c r="F14" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="G14" s="14"/>
+      <c r="H14" s="47"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>5</v>
+      </c>
+      <c r="B15" s="8">
+        <v>60</v>
+      </c>
+      <c r="C15" s="23">
+        <v>140</v>
+      </c>
+      <c r="D15" s="9">
+        <v>1</v>
+      </c>
+      <c r="E15" s="9">
+        <v>0</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G15" s="9"/>
+      <c r="H15" s="10"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>5</v>
+      </c>
+      <c r="B16" s="8">
+        <v>60</v>
+      </c>
+      <c r="C16" s="23">
+        <v>160</v>
+      </c>
+      <c r="D16" s="9">
+        <v>1</v>
+      </c>
+      <c r="E16" s="9">
+        <v>0</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G16" s="9"/>
+      <c r="H16" s="10"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>5</v>
+      </c>
+      <c r="B17" s="8">
+        <v>60</v>
+      </c>
+      <c r="C17" s="23">
+        <v>180</v>
+      </c>
+      <c r="D17" s="9">
+        <v>1</v>
+      </c>
+      <c r="E17" s="9">
+        <v>0</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G17" s="9"/>
+      <c r="H17" s="10"/>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="17">
+        <v>5</v>
+      </c>
+      <c r="B18" s="18">
+        <v>60</v>
+      </c>
+      <c r="C18" s="25">
+        <v>200</v>
+      </c>
+      <c r="D18" s="19">
+        <v>1</v>
+      </c>
+      <c r="E18" s="19">
+        <v>0</v>
+      </c>
+      <c r="F18" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="G18" s="19"/>
+      <c r="H18" s="20"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="50"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="50"/>
+      <c r="H21" s="51"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="40">
+        <v>10</v>
+      </c>
+      <c r="B23" s="24">
+        <v>30</v>
+      </c>
+      <c r="C23" s="24">
+        <v>140</v>
+      </c>
+      <c r="D23" s="30">
+        <v>1</v>
+      </c>
+      <c r="E23" s="30">
+        <v>0</v>
+      </c>
+      <c r="F23" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G23" s="30"/>
+      <c r="H23" s="44"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="40">
+        <v>10</v>
+      </c>
+      <c r="B24" s="24">
+        <v>30</v>
+      </c>
+      <c r="C24" s="24">
+        <v>160</v>
+      </c>
+      <c r="D24" s="30">
+        <v>1</v>
+      </c>
+      <c r="E24" s="30">
+        <v>0</v>
+      </c>
+      <c r="F24" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G24" s="30"/>
+      <c r="H24" s="44"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="40">
+        <v>10</v>
+      </c>
+      <c r="B25" s="24">
+        <v>30</v>
+      </c>
+      <c r="C25" s="24">
+        <v>180</v>
+      </c>
+      <c r="D25" s="30">
+        <v>1</v>
+      </c>
+      <c r="E25" s="30">
+        <v>0</v>
+      </c>
+      <c r="F25" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G25" s="30"/>
+      <c r="H25" s="44"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="40">
+        <v>10</v>
+      </c>
+      <c r="B26" s="24">
+        <v>30</v>
+      </c>
+      <c r="C26" s="24">
+        <v>200</v>
+      </c>
+      <c r="D26" s="30">
+        <v>1</v>
+      </c>
+      <c r="E26" s="30">
+        <v>0</v>
+      </c>
+      <c r="F26" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G26" s="30"/>
+      <c r="H26" s="44"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="41">
+        <v>10</v>
+      </c>
+      <c r="B27" s="23">
+        <v>40</v>
+      </c>
+      <c r="C27" s="23">
+        <v>140</v>
+      </c>
+      <c r="D27" s="32">
+        <v>1</v>
+      </c>
+      <c r="E27" s="32">
+        <v>0</v>
+      </c>
+      <c r="F27" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="G27" s="32"/>
+      <c r="H27" s="45"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="41">
+        <v>10</v>
+      </c>
+      <c r="B28" s="23">
+        <v>40</v>
+      </c>
+      <c r="C28" s="23">
+        <v>160</v>
+      </c>
+      <c r="D28" s="32">
+        <v>1</v>
+      </c>
+      <c r="E28" s="32">
+        <v>0</v>
+      </c>
+      <c r="F28" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="G28" s="32"/>
+      <c r="H28" s="45"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="41">
+        <v>10</v>
+      </c>
+      <c r="B29" s="23">
+        <v>40</v>
+      </c>
+      <c r="C29" s="23">
+        <v>180</v>
+      </c>
+      <c r="D29" s="32">
+        <v>1</v>
+      </c>
+      <c r="E29" s="32">
+        <v>0</v>
+      </c>
+      <c r="F29" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="G29" s="32"/>
+      <c r="H29" s="45"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="41">
+        <v>10</v>
+      </c>
+      <c r="B30" s="23">
+        <v>40</v>
+      </c>
+      <c r="C30" s="23">
+        <v>200</v>
+      </c>
+      <c r="D30" s="32">
+        <v>1</v>
+      </c>
+      <c r="E30" s="32">
+        <v>0</v>
+      </c>
+      <c r="F30" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="G30" s="32"/>
+      <c r="H30" s="45"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="40">
+        <v>10</v>
+      </c>
+      <c r="B31" s="24">
+        <v>50</v>
+      </c>
+      <c r="C31" s="24">
+        <v>140</v>
+      </c>
+      <c r="D31" s="30">
+        <v>1</v>
+      </c>
+      <c r="E31" s="30">
+        <v>0</v>
+      </c>
+      <c r="F31" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G31" s="30"/>
+      <c r="H31" s="44"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="40">
+        <v>10</v>
+      </c>
+      <c r="B32" s="24">
+        <v>50</v>
+      </c>
+      <c r="C32" s="24">
+        <v>160</v>
+      </c>
+      <c r="D32" s="30">
+        <v>1</v>
+      </c>
+      <c r="E32" s="30">
+        <v>0</v>
+      </c>
+      <c r="F32" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G32" s="30"/>
+      <c r="H32" s="44"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="40">
+        <v>10</v>
+      </c>
+      <c r="B33" s="24">
+        <v>50</v>
+      </c>
+      <c r="C33" s="24">
+        <v>180</v>
+      </c>
+      <c r="D33" s="30">
+        <v>1</v>
+      </c>
+      <c r="E33" s="30">
+        <v>0</v>
+      </c>
+      <c r="F33" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G33" s="30"/>
+      <c r="H33" s="44"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="40">
+        <v>10</v>
+      </c>
+      <c r="B34" s="24">
+        <v>50</v>
+      </c>
+      <c r="C34" s="24">
+        <v>200</v>
+      </c>
+      <c r="D34" s="30">
+        <v>1</v>
+      </c>
+      <c r="E34" s="30">
+        <v>0</v>
+      </c>
+      <c r="F34" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="G34" s="30"/>
+      <c r="H34" s="44"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="41">
+        <v>10</v>
+      </c>
+      <c r="B35" s="23">
+        <v>60</v>
+      </c>
+      <c r="C35" s="23">
+        <v>140</v>
+      </c>
+      <c r="D35" s="32">
+        <v>1</v>
+      </c>
+      <c r="E35" s="32">
+        <v>0</v>
+      </c>
+      <c r="F35" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="G35" s="32"/>
+      <c r="H35" s="33"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="41">
+        <v>10</v>
+      </c>
+      <c r="B36" s="23">
+        <v>60</v>
+      </c>
+      <c r="C36" s="23">
+        <v>160</v>
+      </c>
+      <c r="D36" s="32">
+        <v>1</v>
+      </c>
+      <c r="E36" s="32">
+        <v>0</v>
+      </c>
+      <c r="F36" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="G36" s="32"/>
+      <c r="H36" s="33"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="41">
+        <v>10</v>
+      </c>
+      <c r="B37" s="23">
+        <v>60</v>
+      </c>
+      <c r="C37" s="23">
+        <v>180</v>
+      </c>
+      <c r="D37" s="32">
+        <v>1</v>
+      </c>
+      <c r="E37" s="32">
+        <v>0</v>
+      </c>
+      <c r="F37" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="G37" s="32"/>
+      <c r="H37" s="33"/>
+    </row>
+    <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="46">
+        <v>10</v>
+      </c>
+      <c r="B38" s="25">
+        <v>60</v>
+      </c>
+      <c r="C38" s="25">
+        <v>200</v>
+      </c>
+      <c r="D38" s="42">
+        <v>1</v>
+      </c>
+      <c r="E38" s="42">
+        <v>0</v>
+      </c>
+      <c r="F38" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="G38" s="42"/>
+      <c r="H38" s="43"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A21:H21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>